<commit_message>
Updates based on feedback from Kjetil
</commit_message>
<xml_diff>
--- a/data/active_stations_2020.xlsx
+++ b/data/active_stations_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Oeyvind_G\Tiltaksovervakingen\tiltaksovervakingen\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DD064A-A3B2-4ADD-BC41-97518D8CAB69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430D2288-6319-4329-9BC3-A652DA83F69F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="687">
   <si>
     <t>Nidelva/Arendal</t>
   </si>
@@ -1210,12 +1210,6 @@
     <t>Songeelva oppstrøms doserer</t>
   </si>
   <si>
-    <t>Otra oppstrøms doserer</t>
-  </si>
-  <si>
-    <t>Otra nedstrøms doserer</t>
-  </si>
-  <si>
     <t>Langåna v/Røyknes</t>
   </si>
   <si>
@@ -1303,9 +1297,6 @@
     <t>Ny stasjon juli 2020. Ble også prøvetatt under flomepisoder vår-sommer 2019.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ny stasjon juli 2020 </t>
-  </si>
-  <si>
     <t>Kosåna utløp (13)</t>
   </si>
   <si>
@@ -2072,6 +2063,36 @@
   </si>
   <si>
     <t>021-46388</t>
+  </si>
+  <si>
+    <t>019-101022</t>
+  </si>
+  <si>
+    <t>021-101027</t>
+  </si>
+  <si>
+    <t>021-101031</t>
+  </si>
+  <si>
+    <t>021-101033</t>
+  </si>
+  <si>
+    <t>024-101034</t>
+  </si>
+  <si>
+    <t>026-101039</t>
+  </si>
+  <si>
+    <t>Otra nedstrøms doserer Iveland/Kattefoss</t>
+  </si>
+  <si>
+    <t>Otra oppstrøms doserer Iveland (Dalanekilen inntak)</t>
+  </si>
+  <si>
+    <t>Ny stasjon juli 2020 i forbindelse med ny doserer ved Iveland kraftverk. Prøvetas ved kraftverksinntak i Dalanekilen, Gåseflådammen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ny stasjon juli 2020. Prøvetas nedstrøms Kattefossen, ved Røyknesvegen. </t>
   </si>
 </sst>
 </file>
@@ -2114,18 +2135,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2140,7 +2155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2151,7 +2166,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18992,7 +19010,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H224" sqref="H224"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -19012,37 +19030,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
+        <v>665</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>666</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>667</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>668</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="E1" s="6" t="s">
+        <v>671</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>672</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>673</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>674</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>675</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>669</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>670</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>671</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>674</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>675</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>677</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>678</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>672</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
@@ -19053,10 +19071,10 @@
         <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="E2" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="G2" s="7">
         <v>292044.86731100001</v>
@@ -19068,7 +19086,7 @@
         <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
@@ -19079,7 +19097,7 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -19100,7 +19118,7 @@
         <v>33</v>
       </c>
       <c r="J3" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K3" t="s">
         <v>44</v>
@@ -19120,7 +19138,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G4" s="7">
         <v>146117.19357</v>
@@ -19132,10 +19150,10 @@
         <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
@@ -19152,7 +19170,7 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="G5" s="7">
         <v>143490.19312499999</v>
@@ -19164,7 +19182,7 @@
         <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
@@ -19175,13 +19193,13 @@
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D6">
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="G6" s="7">
         <v>143378.37487199999</v>
@@ -19193,10 +19211,10 @@
         <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K6" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
@@ -19228,7 +19246,7 @@
         <v>33</v>
       </c>
       <c r="J7" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
@@ -19245,7 +19263,7 @@
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G8" s="7">
         <v>143345.53039299999</v>
@@ -19257,7 +19275,7 @@
         <v>33</v>
       </c>
       <c r="J8" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
@@ -19274,7 +19292,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="G9" s="7">
         <v>128523.96044900001</v>
@@ -19286,7 +19304,7 @@
         <v>33</v>
       </c>
       <c r="J9" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
@@ -19303,7 +19321,7 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G10" s="7">
         <v>127731.485267</v>
@@ -19315,7 +19333,7 @@
         <v>33</v>
       </c>
       <c r="J10" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K10" t="s">
         <v>7</v>
@@ -19335,7 +19353,7 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G11" s="7">
         <v>112203.512682</v>
@@ -19347,7 +19365,7 @@
         <v>33</v>
       </c>
       <c r="J11" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K11" t="s">
         <v>3</v>
@@ -19367,7 +19385,7 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G12" s="7">
         <v>101429.58238000001</v>
@@ -19379,7 +19397,7 @@
         <v>33</v>
       </c>
       <c r="J12" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K12" t="s">
         <v>5</v>
@@ -19399,7 +19417,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="G13" s="7">
         <v>135135.323378</v>
@@ -19411,7 +19429,7 @@
         <v>33</v>
       </c>
       <c r="J13" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
@@ -19440,7 +19458,7 @@
         <v>33</v>
       </c>
       <c r="J14" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
@@ -19453,7 +19471,9 @@
       <c r="C15" t="s">
         <v>391</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" t="s">
+        <v>677</v>
+      </c>
       <c r="G15" s="7">
         <v>131566</v>
       </c>
@@ -19464,10 +19484,10 @@
         <v>33</v>
       </c>
       <c r="J15" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K15" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
@@ -19478,7 +19498,7 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D16">
         <v>18</v>
@@ -19496,7 +19516,7 @@
         <v>33</v>
       </c>
       <c r="J16" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K16" t="s">
         <v>341</v>
@@ -19510,10 +19530,10 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="E17" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="G17" s="7">
         <v>109017.94520099999</v>
@@ -19525,10 +19545,10 @@
         <v>33</v>
       </c>
       <c r="J17" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K17" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.45">
@@ -19539,10 +19559,10 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="E18" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="G18" s="7">
         <v>108864.263483</v>
@@ -19554,10 +19574,10 @@
         <v>33</v>
       </c>
       <c r="J18" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K18" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
@@ -19574,7 +19594,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G19" s="7">
         <v>97714.164554000003</v>
@@ -19586,7 +19606,7 @@
         <v>33</v>
       </c>
       <c r="J19" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
@@ -19603,7 +19623,7 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G20" s="7">
         <v>110363.331603</v>
@@ -19615,7 +19635,7 @@
         <v>33</v>
       </c>
       <c r="J20" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.45">
@@ -19632,7 +19652,7 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="G21" s="7">
         <v>113473.019562949</v>
@@ -19644,7 +19664,7 @@
         <v>33</v>
       </c>
       <c r="J21" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.45">
@@ -19661,7 +19681,7 @@
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G22" s="7">
         <v>107965.167865</v>
@@ -19673,7 +19693,7 @@
         <v>33</v>
       </c>
       <c r="J22" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
@@ -19705,7 +19725,7 @@
         <v>33</v>
       </c>
       <c r="J23" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K23" t="s">
         <v>30</v>
@@ -19725,7 +19745,7 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="G24" s="7">
         <v>102268.121399</v>
@@ -19737,7 +19757,7 @@
         <v>33</v>
       </c>
       <c r="J24" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.45">
@@ -19769,7 +19789,7 @@
         <v>33</v>
       </c>
       <c r="J25" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.45">
@@ -19795,7 +19815,7 @@
         <v>33</v>
       </c>
       <c r="J26" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K26" t="s">
         <v>342</v>
@@ -19812,10 +19832,10 @@
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="E27" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G27" s="7">
         <v>97590.25232</v>
@@ -19827,7 +19847,7 @@
         <v>33</v>
       </c>
       <c r="J27" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K27" t="s">
         <v>26</v>
@@ -19859,7 +19879,7 @@
         <v>33</v>
       </c>
       <c r="J28" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="K28" t="s">
         <v>383</v>
@@ -19891,7 +19911,7 @@
         <v>33</v>
       </c>
       <c r="J29" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="K29" t="s">
         <v>381</v>
@@ -19905,23 +19925,25 @@
         <v>330</v>
       </c>
       <c r="C30" t="s">
-        <v>604</v>
-      </c>
-      <c r="E30" s="8"/>
+        <v>601</v>
+      </c>
+      <c r="E30" t="s">
+        <v>678</v>
+      </c>
       <c r="G30" s="7">
         <v>83862</v>
       </c>
       <c r="H30" s="7">
         <v>6475878</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="9">
         <v>33</v>
       </c>
       <c r="J30" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K30" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.45">
@@ -19947,7 +19969,7 @@
         <v>33</v>
       </c>
       <c r="J31" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="K31" t="s">
         <v>382</v>
@@ -19961,10 +19983,10 @@
         <v>330</v>
       </c>
       <c r="C32" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E32" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G32" s="7">
         <v>89026</v>
@@ -19976,10 +19998,10 @@
         <v>33</v>
       </c>
       <c r="J32" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K32" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.45">
@@ -19990,10 +20012,10 @@
         <v>330</v>
       </c>
       <c r="C33" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E33" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="G33" s="7">
         <v>84324</v>
@@ -20005,10 +20027,10 @@
         <v>33</v>
       </c>
       <c r="J33" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K33" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.45">
@@ -20034,7 +20056,7 @@
         <v>33</v>
       </c>
       <c r="J34" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K34" t="s">
         <v>385</v>
@@ -20066,7 +20088,7 @@
         <v>33</v>
       </c>
       <c r="J35" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K35" t="s">
         <v>384</v>
@@ -20098,7 +20120,7 @@
         <v>33</v>
       </c>
       <c r="J36" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K36" t="s">
         <v>384</v>
@@ -20112,17 +20134,25 @@
         <v>330</v>
       </c>
       <c r="C37" t="s">
-        <v>393</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
+        <v>683</v>
+      </c>
+      <c r="E37" t="s">
+        <v>680</v>
+      </c>
+      <c r="G37" s="8">
+        <v>85526</v>
+      </c>
+      <c r="H37" s="8">
+        <v>6493180</v>
+      </c>
+      <c r="I37" s="9">
+        <v>33</v>
+      </c>
       <c r="J37" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="K37" t="s">
-        <v>423</v>
+        <v>686</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.45">
@@ -20133,17 +20163,25 @@
         <v>330</v>
       </c>
       <c r="C38" t="s">
-        <v>392</v>
-      </c>
-      <c r="E38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
+        <v>684</v>
+      </c>
+      <c r="E38" t="s">
+        <v>679</v>
+      </c>
+      <c r="G38" s="8">
+        <v>83953</v>
+      </c>
+      <c r="H38" s="8">
+        <v>6495884</v>
+      </c>
+      <c r="I38" s="9">
+        <v>33</v>
+      </c>
       <c r="J38" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K38" t="s">
-        <v>423</v>
+        <v>685</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.45">
@@ -20154,10 +20192,10 @@
         <v>330</v>
       </c>
       <c r="C39" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E39" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G39" s="7">
         <v>76504</v>
@@ -20169,10 +20207,10 @@
         <v>33</v>
       </c>
       <c r="J39" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K39" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.45">
@@ -20198,7 +20236,7 @@
         <v>33</v>
       </c>
       <c r="J40" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K40" t="s">
         <v>50</v>
@@ -20215,7 +20253,7 @@
         <v>52</v>
       </c>
       <c r="E41" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="G41" s="7">
         <v>71614</v>
@@ -20227,7 +20265,7 @@
         <v>33</v>
       </c>
       <c r="J41" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K41" t="s">
         <v>343</v>
@@ -20256,7 +20294,7 @@
         <v>33</v>
       </c>
       <c r="J42" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K42" t="s">
         <v>343</v>
@@ -20285,7 +20323,7 @@
         <v>33</v>
       </c>
       <c r="J43" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K43" t="s">
         <v>343</v>
@@ -20302,7 +20340,7 @@
         <v>321</v>
       </c>
       <c r="E44" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G44" s="7">
         <v>78337.500564999995</v>
@@ -20314,7 +20352,7 @@
         <v>33</v>
       </c>
       <c r="J44" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.45">
@@ -20331,7 +20369,7 @@
         <v>324</v>
       </c>
       <c r="F45" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G45" s="7">
         <v>75109</v>
@@ -20343,7 +20381,7 @@
         <v>33</v>
       </c>
       <c r="J45" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K45" t="s">
         <v>323</v>
@@ -20375,7 +20413,7 @@
         <v>33</v>
       </c>
       <c r="J46" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K46" t="s">
         <v>323</v>
@@ -20395,7 +20433,7 @@
         <v>329</v>
       </c>
       <c r="F47" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="G47" s="7">
         <v>76554</v>
@@ -20407,7 +20445,7 @@
         <v>33</v>
       </c>
       <c r="J47" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K47" t="s">
         <v>323</v>
@@ -20427,7 +20465,7 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="G48" s="7">
         <v>61346.669367000002</v>
@@ -20439,7 +20477,7 @@
         <v>33</v>
       </c>
       <c r="J48" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.45">
@@ -20456,7 +20494,7 @@
         <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="G49" s="7">
         <v>62838.750856999999</v>
@@ -20468,7 +20506,7 @@
         <v>33</v>
       </c>
       <c r="J49" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.45">
@@ -20479,13 +20517,13 @@
         <v>302</v>
       </c>
       <c r="C50" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D50">
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="G50" s="7">
         <v>63676.259080999997</v>
@@ -20497,7 +20535,7 @@
         <v>33</v>
       </c>
       <c r="J50" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.45">
@@ -20523,7 +20561,7 @@
         <v>33</v>
       </c>
       <c r="J51" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K51" t="s">
         <v>376</v>
@@ -20537,13 +20575,13 @@
         <v>302</v>
       </c>
       <c r="C52" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D52">
         <v>11</v>
       </c>
       <c r="E52" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G52" s="7">
         <v>60939.076349000003</v>
@@ -20555,7 +20593,7 @@
         <v>33</v>
       </c>
       <c r="J52" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.45">
@@ -20566,13 +20604,13 @@
         <v>302</v>
       </c>
       <c r="C53" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D53">
         <v>13</v>
       </c>
       <c r="E53" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="G53" s="7">
         <v>64515.144346000001</v>
@@ -20584,7 +20622,7 @@
         <v>33</v>
       </c>
       <c r="J53" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.45">
@@ -20595,13 +20633,13 @@
         <v>302</v>
       </c>
       <c r="C54" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D54">
         <v>15</v>
       </c>
       <c r="E54" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="G54" s="7">
         <v>60469.991418999998</v>
@@ -20613,7 +20651,7 @@
         <v>33</v>
       </c>
       <c r="J54" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.45">
@@ -20639,7 +20677,7 @@
         <v>33</v>
       </c>
       <c r="J55" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K55" t="s">
         <v>377</v>
@@ -20668,7 +20706,7 @@
         <v>33</v>
       </c>
       <c r="J56" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="K56" t="s">
         <v>378</v>
@@ -20703,7 +20741,7 @@
         <v>33</v>
       </c>
       <c r="J57" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.45">
@@ -20735,7 +20773,7 @@
         <v>33</v>
       </c>
       <c r="J58" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.45">
@@ -20752,7 +20790,7 @@
         <v>3</v>
       </c>
       <c r="E59" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="G59" s="7">
         <v>53424.904893999999</v>
@@ -20764,7 +20802,7 @@
         <v>33</v>
       </c>
       <c r="J59" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.45">
@@ -20781,7 +20819,7 @@
         <v>6</v>
       </c>
       <c r="E60" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="G60" s="7">
         <v>49359.760647000003</v>
@@ -20793,7 +20831,7 @@
         <v>33</v>
       </c>
       <c r="J60" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.45">
@@ -20807,10 +20845,10 @@
         <v>281</v>
       </c>
       <c r="D61" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="E61" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="G61" s="7">
         <v>54729.520605999998</v>
@@ -20822,7 +20860,7 @@
         <v>33</v>
       </c>
       <c r="J61" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.45">
@@ -20839,7 +20877,7 @@
         <v>14</v>
       </c>
       <c r="E62" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="G62" s="7">
         <v>50228.873606000001</v>
@@ -20851,7 +20889,7 @@
         <v>33</v>
       </c>
       <c r="J62" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.45">
@@ -20865,10 +20903,10 @@
         <v>278</v>
       </c>
       <c r="D63" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="E63" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="G63" s="7">
         <v>51266.087678999997</v>
@@ -20880,7 +20918,7 @@
         <v>33</v>
       </c>
       <c r="J63" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="K63" t="s">
         <v>373</v>
@@ -20897,10 +20935,10 @@
         <v>279</v>
       </c>
       <c r="D64" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="E64" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="G64" s="7">
         <v>51203</v>
@@ -20912,7 +20950,7 @@
         <v>33</v>
       </c>
       <c r="J64" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="K64" t="s">
         <v>374</v>
@@ -20932,7 +20970,7 @@
         <v>16</v>
       </c>
       <c r="E65" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="G65" s="7">
         <v>51069.624163</v>
@@ -20944,7 +20982,7 @@
         <v>33</v>
       </c>
       <c r="J65" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.45">
@@ -20973,7 +21011,7 @@
         <v>33</v>
       </c>
       <c r="J66" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K66" t="s">
         <v>283</v>
@@ -20993,7 +21031,7 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G67" s="7">
         <v>38898.998094000002</v>
@@ -21005,7 +21043,7 @@
         <v>33</v>
       </c>
       <c r="J67" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.45">
@@ -21022,7 +21060,7 @@
         <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="G68" s="7">
         <v>40591.952972999999</v>
@@ -21034,7 +21072,7 @@
         <v>33</v>
       </c>
       <c r="J68" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.45">
@@ -21051,7 +21089,7 @@
         <v>3</v>
       </c>
       <c r="E69" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G69" s="7">
         <v>44280.163765999998</v>
@@ -21063,7 +21101,7 @@
         <v>33</v>
       </c>
       <c r="J69" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.45">
@@ -21080,7 +21118,7 @@
         <v>4</v>
       </c>
       <c r="E70" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G70" s="7">
         <v>46399.403963999997</v>
@@ -21092,7 +21130,7 @@
         <v>33</v>
       </c>
       <c r="J70" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.45">
@@ -21118,7 +21156,7 @@
         <v>33</v>
       </c>
       <c r="J71" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K71" t="s">
         <v>386</v>
@@ -21132,23 +21170,25 @@
         <v>294</v>
       </c>
       <c r="C72" t="s">
-        <v>397</v>
-      </c>
-      <c r="E72" s="8"/>
+        <v>395</v>
+      </c>
+      <c r="E72" t="s">
+        <v>681</v>
+      </c>
       <c r="G72" s="7">
         <v>33005</v>
       </c>
       <c r="H72" s="7">
         <v>6477280</v>
       </c>
-      <c r="I72" s="7">
+      <c r="I72" s="9">
         <v>33</v>
       </c>
       <c r="J72" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K72" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.45">
@@ -21165,7 +21205,7 @@
         <v>6</v>
       </c>
       <c r="E73" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="G73" s="7">
         <v>33804.067872</v>
@@ -21177,7 +21217,7 @@
         <v>33</v>
       </c>
       <c r="J73" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.45">
@@ -21188,13 +21228,13 @@
         <v>294</v>
       </c>
       <c r="C74" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D74">
         <v>18</v>
       </c>
       <c r="E74" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="G74" s="7">
         <v>40380.618582000003</v>
@@ -21206,7 +21246,7 @@
         <v>33</v>
       </c>
       <c r="J74" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.45">
@@ -21217,13 +21257,13 @@
         <v>294</v>
       </c>
       <c r="C75" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D75">
         <v>19</v>
       </c>
       <c r="E75" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="G75" s="7">
         <v>35691.362739999997</v>
@@ -21235,7 +21275,7 @@
         <v>33</v>
       </c>
       <c r="J75" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.45">
@@ -21252,7 +21292,7 @@
         <v>3</v>
       </c>
       <c r="E76" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="G76" s="7">
         <v>30498.686836000001</v>
@@ -21264,7 +21304,7 @@
         <v>33</v>
       </c>
       <c r="J76" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.45">
@@ -21278,10 +21318,10 @@
         <v>291</v>
       </c>
       <c r="D77" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="E77" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="G77" s="7">
         <v>28114.788872000001</v>
@@ -21293,7 +21333,7 @@
         <v>33</v>
       </c>
       <c r="J77" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.45">
@@ -21304,13 +21344,13 @@
         <v>288</v>
       </c>
       <c r="C78" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D78">
         <v>5</v>
       </c>
       <c r="E78" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="G78" s="7">
         <v>35953.846236999998</v>
@@ -21322,7 +21362,7 @@
         <v>33</v>
       </c>
       <c r="J78" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.45">
@@ -21339,7 +21379,7 @@
         <v>8</v>
       </c>
       <c r="E79" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="G79" s="7">
         <v>30470.752357000001</v>
@@ -21351,7 +21391,7 @@
         <v>33</v>
       </c>
       <c r="J79" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.45">
@@ -21380,7 +21420,7 @@
         <v>33</v>
       </c>
       <c r="J80" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K80" t="s">
         <v>375</v>
@@ -21409,7 +21449,7 @@
         <v>33</v>
       </c>
       <c r="J81" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.45">
@@ -21420,7 +21460,7 @@
         <v>314</v>
       </c>
       <c r="C82" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -21438,7 +21478,7 @@
         <v>33</v>
       </c>
       <c r="J82" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K82" t="s">
         <v>317</v>
@@ -21452,13 +21492,13 @@
         <v>314</v>
       </c>
       <c r="C83" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D83">
         <v>2</v>
       </c>
       <c r="E83" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="G83" s="7">
         <v>-239.22803300000001</v>
@@ -21470,7 +21510,7 @@
         <v>33</v>
       </c>
       <c r="J83" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.45">
@@ -21481,7 +21521,7 @@
         <v>314</v>
       </c>
       <c r="C84" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D84">
         <v>3</v>
@@ -21499,7 +21539,7 @@
         <v>33</v>
       </c>
       <c r="J84" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K84" t="s">
         <v>380</v>
@@ -21528,7 +21568,7 @@
         <v>33</v>
       </c>
       <c r="J85" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K85" t="s">
         <v>379</v>
@@ -21542,13 +21582,13 @@
         <v>190</v>
       </c>
       <c r="C86" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D86">
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="G86" s="7">
         <v>-7923.0859179999998</v>
@@ -21560,10 +21600,10 @@
         <v>33</v>
       </c>
       <c r="J86" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K86" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.45">
@@ -21574,9 +21614,11 @@
         <v>190</v>
       </c>
       <c r="C87" t="s">
-        <v>398</v>
-      </c>
-      <c r="E87" s="8"/>
+        <v>396</v>
+      </c>
+      <c r="E87" t="s">
+        <v>682</v>
+      </c>
       <c r="G87" s="7">
         <v>344012</v>
       </c>
@@ -21587,10 +21629,10 @@
         <v>32</v>
       </c>
       <c r="J87" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K87" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.45">
@@ -21601,13 +21643,13 @@
         <v>190</v>
       </c>
       <c r="C88" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D88">
         <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="G88" s="7">
         <v>-7928.9469600000002</v>
@@ -21619,7 +21661,7 @@
         <v>33</v>
       </c>
       <c r="J88" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.45">
@@ -21630,13 +21672,13 @@
         <v>190</v>
       </c>
       <c r="C89" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D89">
         <v>3</v>
       </c>
       <c r="E89" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="G89" s="7">
         <v>-5753.0666590000001</v>
@@ -21648,7 +21690,7 @@
         <v>33</v>
       </c>
       <c r="J89" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.45">
@@ -21659,13 +21701,13 @@
         <v>190</v>
       </c>
       <c r="C90" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="D90">
         <v>4</v>
       </c>
       <c r="E90" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="G90" s="7">
         <v>-6353.2602809999998</v>
@@ -21677,7 +21719,7 @@
         <v>33</v>
       </c>
       <c r="J90" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.45">
@@ -21688,13 +21730,13 @@
         <v>190</v>
       </c>
       <c r="C91" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D91">
         <v>5</v>
       </c>
       <c r="E91" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="G91" s="7">
         <v>-7669.1387459999996</v>
@@ -21706,7 +21748,7 @@
         <v>33</v>
       </c>
       <c r="J91" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.45">
@@ -21732,7 +21774,7 @@
         <v>33</v>
       </c>
       <c r="J92" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K92" t="s">
         <v>363</v>
@@ -21761,7 +21803,7 @@
         <v>33</v>
       </c>
       <c r="J93" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K93" t="s">
         <v>363</v>
@@ -21793,7 +21835,7 @@
         <v>33</v>
       </c>
       <c r="J94" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K94" t="s">
         <v>364</v>
@@ -21822,7 +21864,7 @@
         <v>33</v>
       </c>
       <c r="J95" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K95" t="s">
         <v>363</v>
@@ -21851,7 +21893,7 @@
         <v>33</v>
       </c>
       <c r="J96" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K96" t="s">
         <v>363</v>
@@ -21883,7 +21925,7 @@
         <v>33</v>
       </c>
       <c r="J97" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K97" t="s">
         <v>365</v>
@@ -21903,7 +21945,7 @@
         <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="G98" s="7">
         <v>-24148.784555999999</v>
@@ -21915,7 +21957,7 @@
         <v>33</v>
       </c>
       <c r="J98" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.45">
@@ -21932,7 +21974,7 @@
         <v>4</v>
       </c>
       <c r="E99" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="G99" s="7">
         <v>-16555.674385999999</v>
@@ -21944,7 +21986,7 @@
         <v>33</v>
       </c>
       <c r="J99" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.45">
@@ -21961,7 +22003,7 @@
         <v>6</v>
       </c>
       <c r="E100" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="G100" s="7">
         <v>865.74685199999999</v>
@@ -21973,7 +22015,7 @@
         <v>33</v>
       </c>
       <c r="J100" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.45">
@@ -21990,7 +22032,7 @@
         <v>7</v>
       </c>
       <c r="E101" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="G101" s="7">
         <v>1688.192515</v>
@@ -22002,7 +22044,7 @@
         <v>33</v>
       </c>
       <c r="J101" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.45">
@@ -22019,7 +22061,7 @@
         <v>8</v>
       </c>
       <c r="E102" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="G102" s="7">
         <v>-7748.0731370000003</v>
@@ -22031,7 +22073,7 @@
         <v>33</v>
       </c>
       <c r="J102" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.45">
@@ -22048,7 +22090,7 @@
         <v>9</v>
       </c>
       <c r="E103" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G103" s="7">
         <v>-11817.160059</v>
@@ -22060,7 +22102,7 @@
         <v>33</v>
       </c>
       <c r="J103" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.45">
@@ -22077,7 +22119,7 @@
         <v>12</v>
       </c>
       <c r="E104" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="G104" s="7">
         <v>-15325.023718</v>
@@ -22089,7 +22131,7 @@
         <v>33</v>
       </c>
       <c r="J104" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.45">
@@ -22106,7 +22148,7 @@
         <v>14</v>
       </c>
       <c r="E105" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="G105" s="7">
         <v>-9237.6714699999993</v>
@@ -22118,7 +22160,7 @@
         <v>33</v>
       </c>
       <c r="J105" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K105" t="s">
         <v>147</v>
@@ -22138,7 +22180,7 @@
         <v>15</v>
       </c>
       <c r="E106" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="G106" s="7">
         <v>-9693.6067800000001</v>
@@ -22150,7 +22192,7 @@
         <v>33</v>
       </c>
       <c r="J106" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K106" t="s">
         <v>145</v>
@@ -22164,13 +22206,13 @@
         <v>175</v>
       </c>
       <c r="C107" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D107">
         <v>4</v>
       </c>
       <c r="E107" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="G107" s="7">
         <v>-32671.270689000001</v>
@@ -22182,10 +22224,10 @@
         <v>33</v>
       </c>
       <c r="J107" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K107" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.45">
@@ -22202,7 +22244,7 @@
         <v>48</v>
       </c>
       <c r="E108" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="G108" s="7">
         <v>-21333.146041</v>
@@ -22214,10 +22256,10 @@
         <v>33</v>
       </c>
       <c r="J108" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K108" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.45">
@@ -22234,7 +22276,7 @@
         <v>50</v>
       </c>
       <c r="E109" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="G109" s="7">
         <v>-23756.366348</v>
@@ -22246,7 +22288,7 @@
         <v>33</v>
       </c>
       <c r="J109" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.45">
@@ -22263,7 +22305,7 @@
         <v>51</v>
       </c>
       <c r="E110" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="G110" s="7">
         <v>-23746.894015999998</v>
@@ -22275,7 +22317,7 @@
         <v>33</v>
       </c>
       <c r="J110" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.45">
@@ -22292,7 +22334,7 @@
         <v>52</v>
       </c>
       <c r="E111" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="G111" s="7">
         <v>-32698.885877000001</v>
@@ -22304,10 +22346,10 @@
         <v>33</v>
       </c>
       <c r="J111" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K111" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.45">
@@ -22318,7 +22360,7 @@
         <v>175</v>
       </c>
       <c r="C112" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D112">
         <v>53</v>
@@ -22339,10 +22381,10 @@
         <v>33</v>
       </c>
       <c r="J112" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K112" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.45">
@@ -22359,7 +22401,7 @@
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="G113" s="7">
         <v>-967.01564800000006</v>
@@ -22371,7 +22413,7 @@
         <v>33</v>
       </c>
       <c r="J113" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K113" t="s">
         <v>166</v>
@@ -22385,16 +22427,16 @@
         <v>159</v>
       </c>
       <c r="C114" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D114">
         <v>2</v>
       </c>
       <c r="E114" t="s">
+        <v>500</v>
+      </c>
+      <c r="F114" t="s">
         <v>503</v>
-      </c>
-      <c r="F114" t="s">
-        <v>506</v>
       </c>
       <c r="G114" s="7">
         <v>2426.211605</v>
@@ -22406,7 +22448,7 @@
         <v>33</v>
       </c>
       <c r="J114" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K114" t="s">
         <v>160</v>
@@ -22441,7 +22483,7 @@
         <v>33</v>
       </c>
       <c r="J115" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K115" t="s">
         <v>162</v>
@@ -22455,16 +22497,16 @@
         <v>159</v>
       </c>
       <c r="C116" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D116">
         <v>4</v>
       </c>
       <c r="E116" t="s">
+        <v>501</v>
+      </c>
+      <c r="F116" t="s">
         <v>504</v>
-      </c>
-      <c r="F116" t="s">
-        <v>507</v>
       </c>
       <c r="G116" s="7">
         <v>2589.447658</v>
@@ -22476,7 +22518,7 @@
         <v>33</v>
       </c>
       <c r="J116" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K116" t="s">
         <v>356</v>
@@ -22490,16 +22532,16 @@
         <v>159</v>
       </c>
       <c r="C117" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D117">
         <v>5</v>
       </c>
       <c r="E117" t="s">
+        <v>502</v>
+      </c>
+      <c r="F117" t="s">
         <v>505</v>
-      </c>
-      <c r="F117" t="s">
-        <v>508</v>
       </c>
       <c r="G117" s="7">
         <v>3231.5613589999998</v>
@@ -22511,7 +22553,7 @@
         <v>33</v>
       </c>
       <c r="J117" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="K117" t="s">
         <v>357</v>
@@ -22528,10 +22570,10 @@
         <v>158</v>
       </c>
       <c r="D118" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="E118" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="G118" s="7">
         <v>-435.61006500000002</v>
@@ -22543,7 +22585,7 @@
         <v>33</v>
       </c>
       <c r="J118" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.45">
@@ -22560,7 +22602,7 @@
         <v>1</v>
       </c>
       <c r="E119" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="G119" s="7">
         <v>-445.99656299999998</v>
@@ -22572,7 +22614,7 @@
         <v>33</v>
       </c>
       <c r="J119" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K119" t="s">
         <v>157</v>
@@ -22592,7 +22634,7 @@
         <v>3</v>
       </c>
       <c r="E120" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="G120" s="7">
         <v>-4131.4289749999998</v>
@@ -22604,7 +22646,7 @@
         <v>33</v>
       </c>
       <c r="J120" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.45">
@@ -22621,7 +22663,7 @@
         <v>5</v>
       </c>
       <c r="E121" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="G121" s="7">
         <v>-9405.6402849999995</v>
@@ -22633,7 +22675,7 @@
         <v>33</v>
       </c>
       <c r="J121" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.45">
@@ -22650,7 +22692,7 @@
         <v>6</v>
       </c>
       <c r="E122" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="G122" s="7">
         <v>847.46973000000003</v>
@@ -22662,7 +22704,7 @@
         <v>33</v>
       </c>
       <c r="J122" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.45">
@@ -22673,13 +22715,13 @@
         <v>172</v>
       </c>
       <c r="C123" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D123">
         <v>1</v>
       </c>
       <c r="E123" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="G123" s="7">
         <v>24767.383523</v>
@@ -22691,7 +22733,7 @@
         <v>33</v>
       </c>
       <c r="J123" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.45">
@@ -22702,13 +22744,13 @@
         <v>172</v>
       </c>
       <c r="C124" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D124">
         <v>3</v>
       </c>
       <c r="E124" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="G124" s="7">
         <v>22269.240881000002</v>
@@ -22720,7 +22762,7 @@
         <v>33</v>
       </c>
       <c r="J124" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.45">
@@ -22731,13 +22773,13 @@
         <v>172</v>
       </c>
       <c r="C125" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D125">
         <v>4</v>
       </c>
       <c r="E125" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="G125" s="7">
         <v>22042.742042999998</v>
@@ -22749,7 +22791,7 @@
         <v>33</v>
       </c>
       <c r="J125" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K125" t="s">
         <v>174</v>
@@ -22769,7 +22811,7 @@
         <v>7</v>
       </c>
       <c r="E126" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="G126" s="7">
         <v>23098.613496999998</v>
@@ -22781,7 +22823,7 @@
         <v>33</v>
       </c>
       <c r="J126" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.45">
@@ -22795,7 +22837,7 @@
         <v>168</v>
       </c>
       <c r="D127" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E127" t="s">
         <v>169</v>
@@ -22813,10 +22855,10 @@
         <v>33</v>
       </c>
       <c r="J127" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K127" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.45">
@@ -22833,7 +22875,7 @@
         <v>4</v>
       </c>
       <c r="E128" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="G128" s="7">
         <v>-13128.407453</v>
@@ -22845,7 +22887,7 @@
         <v>33</v>
       </c>
       <c r="J128" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.45">
@@ -22856,7 +22898,7 @@
         <v>206</v>
       </c>
       <c r="C129" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D129">
         <v>11</v>
@@ -22874,7 +22916,7 @@
         <v>33</v>
       </c>
       <c r="J129" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.45">
@@ -22885,7 +22927,7 @@
         <v>206</v>
       </c>
       <c r="C130" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D130">
         <v>12</v>
@@ -22903,7 +22945,7 @@
         <v>33</v>
       </c>
       <c r="J130" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K130" t="s">
         <v>366</v>
@@ -22935,7 +22977,7 @@
         <v>33</v>
       </c>
       <c r="J131" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.45">
@@ -22946,7 +22988,7 @@
         <v>206</v>
       </c>
       <c r="C132" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D132">
         <v>14</v>
@@ -22964,7 +23006,7 @@
         <v>33</v>
       </c>
       <c r="J132" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.45">
@@ -22993,7 +23035,7 @@
         <v>33</v>
       </c>
       <c r="J133" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.45">
@@ -23022,7 +23064,7 @@
         <v>33</v>
       </c>
       <c r="J134" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K134" t="s">
         <v>367</v>
@@ -23039,7 +23081,7 @@
         <v>224</v>
       </c>
       <c r="D135" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="E135" t="s">
         <v>225</v>
@@ -23054,7 +23096,7 @@
         <v>33</v>
       </c>
       <c r="J135" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.45">
@@ -23068,7 +23110,7 @@
         <v>222</v>
       </c>
       <c r="D136" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="E136" t="s">
         <v>223</v>
@@ -23083,7 +23125,7 @@
         <v>33</v>
       </c>
       <c r="J136" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.45">
@@ -23097,7 +23139,7 @@
         <v>218</v>
       </c>
       <c r="D137" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="E137" t="s">
         <v>219</v>
@@ -23112,7 +23154,7 @@
         <v>33</v>
       </c>
       <c r="J137" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.45">
@@ -23126,7 +23168,7 @@
         <v>216</v>
       </c>
       <c r="D138" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E138" t="s">
         <v>217</v>
@@ -23141,7 +23183,7 @@
         <v>33</v>
       </c>
       <c r="J138" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.45">
@@ -23155,7 +23197,7 @@
         <v>207</v>
       </c>
       <c r="D139" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="E139" t="s">
         <v>208</v>
@@ -23170,7 +23212,7 @@
         <v>33</v>
       </c>
       <c r="J139" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.45">
@@ -23181,10 +23223,10 @@
         <v>206</v>
       </c>
       <c r="C140" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D140" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="E140" t="s">
         <v>226</v>
@@ -23199,7 +23241,7 @@
         <v>33</v>
       </c>
       <c r="J140" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K140" t="s">
         <v>368</v>
@@ -23213,10 +23255,10 @@
         <v>206</v>
       </c>
       <c r="C141" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D141" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="E141" t="s">
         <v>227</v>
@@ -23231,7 +23273,7 @@
         <v>33</v>
       </c>
       <c r="J141" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K141" t="s">
         <v>369</v>
@@ -23245,10 +23287,10 @@
         <v>206</v>
       </c>
       <c r="C142" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D142" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="E142" t="s">
         <v>228</v>
@@ -23263,7 +23305,7 @@
         <v>33</v>
       </c>
       <c r="J142" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K142" t="s">
         <v>247</v>
@@ -23280,10 +23322,10 @@
         <v>236</v>
       </c>
       <c r="D143" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="E143" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="G143" s="7">
         <v>-13388.353966000001</v>
@@ -23295,7 +23337,7 @@
         <v>33</v>
       </c>
       <c r="J143" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.45">
@@ -23309,7 +23351,7 @@
         <v>233</v>
       </c>
       <c r="D144" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="E144" t="s">
         <v>234</v>
@@ -23327,10 +23369,10 @@
         <v>32</v>
       </c>
       <c r="J144" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K144" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.45">
@@ -23344,10 +23386,10 @@
         <v>232</v>
       </c>
       <c r="D145" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="E145" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="G145" s="7">
         <v>-10380.171338</v>
@@ -23359,7 +23401,7 @@
         <v>33</v>
       </c>
       <c r="J145" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.45">
@@ -23373,10 +23415,10 @@
         <v>231</v>
       </c>
       <c r="D146" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E146" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G146" s="7">
         <v>-9248.3661780000002</v>
@@ -23388,7 +23430,7 @@
         <v>33</v>
       </c>
       <c r="J146" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.45">
@@ -23402,10 +23444,10 @@
         <v>230</v>
       </c>
       <c r="D147" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E147" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="G147" s="7">
         <v>-9339.310442</v>
@@ -23417,7 +23459,7 @@
         <v>33</v>
       </c>
       <c r="J147" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.45">
@@ -23428,10 +23470,10 @@
         <v>229</v>
       </c>
       <c r="C148" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D148" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="E148" t="s">
         <v>237</v>
@@ -23446,7 +23488,7 @@
         <v>33</v>
       </c>
       <c r="J148" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K148" t="s">
         <v>370</v>
@@ -23463,7 +23505,7 @@
         <v>360</v>
       </c>
       <c r="D149" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E149" t="s">
         <v>186</v>
@@ -23481,7 +23523,7 @@
         <v>33</v>
       </c>
       <c r="J149" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K149" t="s">
         <v>361</v>
@@ -23498,7 +23540,7 @@
         <v>188</v>
       </c>
       <c r="D150" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="E150" t="s">
         <v>189</v>
@@ -23513,7 +23555,7 @@
         <v>33</v>
       </c>
       <c r="J150" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K150" t="s">
         <v>362</v>
@@ -23530,7 +23572,7 @@
         <v>359</v>
       </c>
       <c r="D151" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="E151" t="s">
         <v>185</v>
@@ -23545,7 +23587,7 @@
         <v>33</v>
       </c>
       <c r="J151" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K151" t="s">
         <v>358</v>
@@ -23562,13 +23604,13 @@
         <v>183</v>
       </c>
       <c r="D152" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="E152" t="s">
         <v>184</v>
       </c>
       <c r="F152" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="G152" s="7">
         <v>-15236</v>
@@ -23580,10 +23622,10 @@
         <v>33</v>
       </c>
       <c r="J152" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K152" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.45">
@@ -23594,16 +23636,16 @@
         <v>93</v>
       </c>
       <c r="C153" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D153" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="E153" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F153" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="G153" s="7">
         <v>-9606.8189999999995</v>
@@ -23615,7 +23657,7 @@
         <v>33</v>
       </c>
       <c r="J153" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.45">
@@ -23626,16 +23668,16 @@
         <v>93</v>
       </c>
       <c r="C154" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D154" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="E154" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F154" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="G154" s="7">
         <v>-7081.4575999999997</v>
@@ -23647,7 +23689,7 @@
         <v>33</v>
       </c>
       <c r="J154" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.45">
@@ -23658,16 +23700,16 @@
         <v>93</v>
       </c>
       <c r="C155" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D155" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="E155" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="F155" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="G155" s="7">
         <v>-7682.8486999999996</v>
@@ -23679,10 +23721,10 @@
         <v>33</v>
       </c>
       <c r="J155" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K155" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.45">
@@ -23693,16 +23735,16 @@
         <v>93</v>
       </c>
       <c r="C156" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D156" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="E156" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="F156" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="G156" s="7">
         <v>-7941.6787000000004</v>
@@ -23714,10 +23756,10 @@
         <v>33</v>
       </c>
       <c r="J156" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K156" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.45">
@@ -23731,7 +23773,7 @@
         <v>89</v>
       </c>
       <c r="E157" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="G157" s="7">
         <v>-1511.7375999999999</v>
@@ -23743,7 +23785,7 @@
         <v>33</v>
       </c>
       <c r="J157" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.45">
@@ -23757,7 +23799,7 @@
         <v>88</v>
       </c>
       <c r="E158" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="G158" s="7">
         <v>205.46729999999999</v>
@@ -23769,7 +23811,7 @@
         <v>33</v>
       </c>
       <c r="J158" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.45">
@@ -23783,10 +23825,10 @@
         <v>90</v>
       </c>
       <c r="D159" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="E159" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="G159" s="7">
         <v>-5621.3424999999997</v>
@@ -23798,7 +23840,7 @@
         <v>33</v>
       </c>
       <c r="J159" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.45">
@@ -23812,10 +23854,10 @@
         <v>91</v>
       </c>
       <c r="D160" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E160" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="G160" s="7">
         <v>-5808.415</v>
@@ -23827,7 +23869,7 @@
         <v>33</v>
       </c>
       <c r="J160" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K160" t="s">
         <v>344</v>
@@ -23844,10 +23886,10 @@
         <v>92</v>
       </c>
       <c r="D161" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E161" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="G161" s="7">
         <v>-7743.46</v>
@@ -23859,7 +23901,7 @@
         <v>33</v>
       </c>
       <c r="J161" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.45">
@@ -23873,10 +23915,10 @@
         <v>60</v>
       </c>
       <c r="D162" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="E162" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="G162" s="7">
         <v>-1325.5878</v>
@@ -23888,7 +23930,7 @@
         <v>33</v>
       </c>
       <c r="J162" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.45">
@@ -23902,10 +23944,10 @@
         <v>61</v>
       </c>
       <c r="D163" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E163" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="G163" s="7">
         <v>-2308.2676999999999</v>
@@ -23917,7 +23959,7 @@
         <v>33</v>
       </c>
       <c r="J163" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.45">
@@ -23931,10 +23973,10 @@
         <v>97</v>
       </c>
       <c r="D164" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="E164" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="G164" s="7">
         <v>37414.972500000003</v>
@@ -23946,7 +23988,7 @@
         <v>33</v>
       </c>
       <c r="J164" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.45">
@@ -23960,10 +24002,10 @@
         <v>98</v>
       </c>
       <c r="D165" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E165" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="G165" s="7">
         <v>32589.801899999999</v>
@@ -23975,7 +24017,7 @@
         <v>33</v>
       </c>
       <c r="J165" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.45">
@@ -23989,10 +24031,10 @@
         <v>96</v>
       </c>
       <c r="D166" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E166" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="G166" s="7">
         <v>17092.468199999999</v>
@@ -24004,7 +24046,7 @@
         <v>33</v>
       </c>
       <c r="J166" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.45">
@@ -24018,10 +24060,10 @@
         <v>99</v>
       </c>
       <c r="D167" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="E167" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="G167" s="7">
         <v>14021.164199999999</v>
@@ -24033,7 +24075,7 @@
         <v>33</v>
       </c>
       <c r="J167" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.45">
@@ -24047,10 +24089,10 @@
         <v>95</v>
       </c>
       <c r="D168" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="E168" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="G168" s="7">
         <v>6492.1962000000003</v>
@@ -24062,7 +24104,7 @@
         <v>33</v>
       </c>
       <c r="J168" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.45">
@@ -24076,10 +24118,10 @@
         <v>100</v>
       </c>
       <c r="D169" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="E169" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="G169" s="7">
         <v>14581.5694</v>
@@ -24091,7 +24133,7 @@
         <v>33</v>
       </c>
       <c r="J169" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.45">
@@ -24102,16 +24144,16 @@
         <v>94</v>
       </c>
       <c r="C170" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="D170">
         <v>10</v>
       </c>
       <c r="E170" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F170" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="G170" s="7">
         <v>14174.4043</v>
@@ -24123,7 +24165,7 @@
         <v>33</v>
       </c>
       <c r="J170" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.45">
@@ -24137,7 +24179,7 @@
         <v>69</v>
       </c>
       <c r="D171" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="E171" t="s">
         <v>70</v>
@@ -24155,7 +24197,7 @@
         <v>33</v>
       </c>
       <c r="J171" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.45">
@@ -24169,7 +24211,7 @@
         <v>81</v>
       </c>
       <c r="D172" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="E172" t="s">
         <v>83</v>
@@ -24187,7 +24229,7 @@
         <v>33</v>
       </c>
       <c r="J172" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K172" t="s">
         <v>82</v>
@@ -24204,7 +24246,7 @@
         <v>75</v>
       </c>
       <c r="D173" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E173" t="s">
         <v>76</v>
@@ -24222,7 +24264,7 @@
         <v>33</v>
       </c>
       <c r="J173" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.45">
@@ -24236,7 +24278,7 @@
         <v>63</v>
       </c>
       <c r="D174" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E174" t="s">
         <v>64</v>
@@ -24254,7 +24296,7 @@
         <v>33</v>
       </c>
       <c r="J174" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.45">
@@ -24268,7 +24310,7 @@
         <v>66</v>
       </c>
       <c r="D175" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E175" t="s">
         <v>67</v>
@@ -24286,7 +24328,7 @@
         <v>33</v>
       </c>
       <c r="J175" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.45">
@@ -24300,7 +24342,7 @@
         <v>78</v>
       </c>
       <c r="D176" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E176" t="s">
         <v>79</v>
@@ -24318,7 +24360,7 @@
         <v>33</v>
       </c>
       <c r="J176" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.45">
@@ -24332,7 +24374,7 @@
         <v>85</v>
       </c>
       <c r="D177" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E177" t="s">
         <v>86</v>
@@ -24350,7 +24392,7 @@
         <v>33</v>
       </c>
       <c r="J177" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.45">
@@ -24364,7 +24406,7 @@
         <v>72</v>
       </c>
       <c r="D178" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="E178" t="s">
         <v>73</v>
@@ -24382,7 +24424,7 @@
         <v>33</v>
       </c>
       <c r="J178" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.45">
@@ -24393,10 +24435,10 @@
         <v>128</v>
       </c>
       <c r="C179" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D179" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="E179" t="s">
         <v>129</v>
@@ -24414,7 +24456,7 @@
         <v>33</v>
       </c>
       <c r="J179" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K179" t="s">
         <v>352</v>
@@ -24428,10 +24470,10 @@
         <v>128</v>
       </c>
       <c r="C180" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="D180" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E180" t="s">
         <v>132</v>
@@ -24446,7 +24488,7 @@
         <v>33</v>
       </c>
       <c r="J180" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K180" t="s">
         <v>131</v>
@@ -24460,10 +24502,10 @@
         <v>128</v>
       </c>
       <c r="C181" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="D181" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E181" t="s">
         <v>134</v>
@@ -24481,7 +24523,7 @@
         <v>33</v>
       </c>
       <c r="J181" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K181" t="s">
         <v>354</v>
@@ -24495,10 +24537,10 @@
         <v>128</v>
       </c>
       <c r="C182" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D182" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E182" t="s">
         <v>133</v>
@@ -24513,7 +24555,7 @@
         <v>33</v>
       </c>
       <c r="J182" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K182" t="s">
         <v>353</v>
@@ -24527,10 +24569,10 @@
         <v>128</v>
       </c>
       <c r="C183" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="D183" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E183" t="s">
         <v>136</v>
@@ -24545,7 +24587,7 @@
         <v>33</v>
       </c>
       <c r="J183" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K183" t="s">
         <v>131</v>
@@ -24559,10 +24601,10 @@
         <v>128</v>
       </c>
       <c r="C184" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="D184" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="E184" t="s">
         <v>137</v>
@@ -24580,7 +24622,7 @@
         <v>33</v>
       </c>
       <c r="J184" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K184" t="s">
         <v>355</v>
@@ -24612,7 +24654,7 @@
         <v>33</v>
       </c>
       <c r="J185" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K185" t="s">
         <v>82</v>
@@ -24641,7 +24683,7 @@
         <v>33</v>
       </c>
       <c r="J186" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K186" t="s">
         <v>82</v>
@@ -24673,7 +24715,7 @@
         <v>33</v>
       </c>
       <c r="J187" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K187" t="s">
         <v>82</v>
@@ -24690,7 +24732,7 @@
         <v>106</v>
       </c>
       <c r="D188" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="E188" t="s">
         <v>107</v>
@@ -24705,7 +24747,7 @@
         <v>33</v>
       </c>
       <c r="J188" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K188" t="s">
         <v>347</v>
@@ -24722,7 +24764,7 @@
         <v>108</v>
       </c>
       <c r="D189" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E189" t="s">
         <v>109</v>
@@ -24737,7 +24779,7 @@
         <v>33</v>
       </c>
       <c r="J189" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K189" t="s">
         <v>347</v>
@@ -24754,7 +24796,7 @@
         <v>110</v>
       </c>
       <c r="D190" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E190" t="s">
         <v>111</v>
@@ -24769,7 +24811,7 @@
         <v>33</v>
       </c>
       <c r="J190" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K190" t="s">
         <v>347</v>
@@ -24786,7 +24828,7 @@
         <v>112</v>
       </c>
       <c r="D191" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E191" t="s">
         <v>113</v>
@@ -24801,7 +24843,7 @@
         <v>33</v>
       </c>
       <c r="J191" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K191" t="s">
         <v>347</v>
@@ -24818,7 +24860,7 @@
         <v>115</v>
       </c>
       <c r="D192" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="E192" t="s">
         <v>116</v>
@@ -24833,7 +24875,7 @@
         <v>33</v>
       </c>
       <c r="J192" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K192" t="s">
         <v>347</v>
@@ -24850,7 +24892,7 @@
         <v>117</v>
       </c>
       <c r="D193" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E193" t="s">
         <v>118</v>
@@ -24865,7 +24907,7 @@
         <v>33</v>
       </c>
       <c r="J193" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K193" t="s">
         <v>347</v>
@@ -24882,7 +24924,7 @@
         <v>119</v>
       </c>
       <c r="D194" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E194" t="s">
         <v>120</v>
@@ -24897,7 +24939,7 @@
         <v>33</v>
       </c>
       <c r="J194" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K194" t="s">
         <v>347</v>
@@ -24914,10 +24956,10 @@
         <v>103</v>
       </c>
       <c r="D195" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E195" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="G195" s="7">
         <v>-22737.912199999999</v>
@@ -24929,7 +24971,7 @@
         <v>33</v>
       </c>
       <c r="J195" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K195" t="s">
         <v>350</v>
@@ -24946,10 +24988,10 @@
         <v>102</v>
       </c>
       <c r="D196" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E196" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="G196" s="7">
         <v>-27117.159599999999</v>
@@ -24961,7 +25003,7 @@
         <v>33</v>
       </c>
       <c r="J196" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.45">
@@ -24975,10 +25017,10 @@
         <v>101</v>
       </c>
       <c r="D197" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="E197" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="G197" s="7">
         <v>-27524.878000000001</v>
@@ -24990,7 +25032,7 @@
         <v>33</v>
       </c>
       <c r="J197" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.45">
@@ -25001,13 +25043,13 @@
         <v>390</v>
       </c>
       <c r="C198" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="D198" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E198" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="G198" s="7">
         <v>-30216.382900000001</v>
@@ -25019,7 +25061,7 @@
         <v>33</v>
       </c>
       <c r="J198" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K198" t="s">
         <v>349</v>
@@ -25033,13 +25075,13 @@
         <v>390</v>
       </c>
       <c r="C199" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D199" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="E199" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="G199" s="7">
         <v>-30401.414799999999</v>
@@ -25051,10 +25093,10 @@
         <v>33</v>
       </c>
       <c r="J199" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K199" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.45">
@@ -25068,7 +25110,7 @@
         <v>346</v>
       </c>
       <c r="D200" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="E200" t="s">
         <v>104</v>
@@ -25083,7 +25125,7 @@
         <v>33</v>
       </c>
       <c r="J200" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K200" t="s">
         <v>345</v>
@@ -25097,13 +25139,13 @@
         <v>390</v>
       </c>
       <c r="C201" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D201" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="E201" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="G201" s="7">
         <v>-24672.011399999999</v>
@@ -25115,10 +25157,10 @@
         <v>33</v>
       </c>
       <c r="J201" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K201" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.45">
@@ -25132,10 +25174,10 @@
         <v>259</v>
       </c>
       <c r="E202" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F202" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="G202" s="7">
         <v>26158.044693</v>
@@ -25147,7 +25189,7 @@
         <v>33</v>
       </c>
       <c r="J202" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K202" t="s">
         <v>260</v>
@@ -25164,10 +25206,10 @@
         <v>261</v>
       </c>
       <c r="E203" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="F203" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="G203" s="7">
         <v>26065.148562999999</v>
@@ -25179,7 +25221,7 @@
         <v>33</v>
       </c>
       <c r="J203" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K203" t="s">
         <v>262</v>
@@ -25196,10 +25238,10 @@
         <v>263</v>
       </c>
       <c r="E204" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="F204" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="G204" s="7">
         <v>26116.073284999999</v>
@@ -25211,7 +25253,7 @@
         <v>33</v>
       </c>
       <c r="J204" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K204" t="s">
         <v>372</v>
@@ -25228,10 +25270,10 @@
         <v>264</v>
       </c>
       <c r="E205" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="F205" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="G205" s="7">
         <v>21795.243349</v>
@@ -25243,7 +25285,7 @@
         <v>33</v>
       </c>
       <c r="J205" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K205" t="s">
         <v>265</v>
@@ -25260,10 +25302,10 @@
         <v>266</v>
       </c>
       <c r="E206" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="F206" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="G206" s="7">
         <v>24700.341451</v>
@@ -25275,7 +25317,7 @@
         <v>33</v>
       </c>
       <c r="J206" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.45">
@@ -25304,7 +25346,7 @@
         <v>33</v>
       </c>
       <c r="J207" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K207" t="s">
         <v>268</v>
@@ -25321,10 +25363,10 @@
         <v>248</v>
       </c>
       <c r="D208" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E208" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="G208" s="7">
         <v>-5382.4546069999997</v>
@@ -25336,7 +25378,7 @@
         <v>33</v>
       </c>
       <c r="J208" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.45">
@@ -25350,10 +25392,10 @@
         <v>251</v>
       </c>
       <c r="D209" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E209" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="G209" s="7">
         <v>-5863.5875050000004</v>
@@ -25365,7 +25407,7 @@
         <v>33</v>
       </c>
       <c r="J209" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K209" t="s">
         <v>252</v>
@@ -25379,16 +25421,16 @@
         <v>238</v>
       </c>
       <c r="C210" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="D210" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E210" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="F210" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="G210" s="7">
         <v>-6692</v>
@@ -25400,10 +25442,10 @@
         <v>33</v>
       </c>
       <c r="J210" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K210" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.45">
@@ -25417,10 +25459,10 @@
         <v>246</v>
       </c>
       <c r="D211" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E211" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="G211" s="7">
         <v>-16184.035458</v>
@@ -25432,7 +25474,7 @@
         <v>33</v>
       </c>
       <c r="J211" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="K211" t="s">
         <v>247</v>
@@ -25449,10 +25491,10 @@
         <v>244</v>
       </c>
       <c r="D212" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="E212" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="G212" s="7">
         <v>-14821.784298</v>
@@ -25464,7 +25506,7 @@
         <v>33</v>
       </c>
       <c r="J212" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K212" t="s">
         <v>245</v>
@@ -25481,10 +25523,10 @@
         <v>241</v>
       </c>
       <c r="D213" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E213" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="G213" s="7">
         <v>-17974.03659</v>
@@ -25496,7 +25538,7 @@
         <v>33</v>
       </c>
       <c r="J213" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K213" t="s">
         <v>242</v>
@@ -25513,10 +25555,10 @@
         <v>239</v>
       </c>
       <c r="D214" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="E214" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="G214" s="7">
         <v>-16699.671394000001</v>
@@ -25528,7 +25570,7 @@
         <v>33</v>
       </c>
       <c r="J214" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K214" t="s">
         <v>240</v>
@@ -25545,10 +25587,10 @@
         <v>249</v>
       </c>
       <c r="D215" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="E215" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="G215" s="7">
         <v>-15587.081733000001</v>
@@ -25560,7 +25602,7 @@
         <v>33</v>
       </c>
       <c r="J215" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K215" t="s">
         <v>250</v>
@@ -25577,10 +25619,10 @@
         <v>243</v>
       </c>
       <c r="D216" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="E216" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="G216" s="7">
         <v>-14532.244757</v>
@@ -25592,7 +25634,7 @@
         <v>33</v>
       </c>
       <c r="J216" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="217" spans="1:11" x14ac:dyDescent="0.45">
@@ -25606,7 +25648,7 @@
         <v>255</v>
       </c>
       <c r="D217" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="E217" t="s">
         <v>256</v>
@@ -25621,7 +25663,7 @@
         <v>33</v>
       </c>
       <c r="J217" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K217" t="s">
         <v>371</v>
@@ -25638,7 +25680,7 @@
         <v>253</v>
       </c>
       <c r="D218" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="E218" t="s">
         <v>254</v>
@@ -25653,7 +25695,7 @@
         <v>33</v>
       </c>
       <c r="J218" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K218" t="s">
         <v>371</v>
@@ -25670,7 +25712,7 @@
         <v>257</v>
       </c>
       <c r="D219" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="E219" t="s">
         <v>258</v>
@@ -25685,7 +25727,7 @@
         <v>33</v>
       </c>
       <c r="J219" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K219" t="s">
         <v>371</v>
@@ -25699,11 +25741,52 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="f3010fb3-0ead-40f9-8418-3186255a05f9" ContentTypeId="0x010100D14BD004BF1C4459B890F3727F092580" PreviousValue="false"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <gdc15e87e6184dc285cecc59dfe3e409 xmlns="99b93dda-0db1-4804-bcd9-79ac3408f7b3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </gdc15e87e6184dc285cecc59dfe3e409>
+    <TaxCatchAll xmlns="99b93dda-0db1-4804-bcd9-79ac3408f7b3">
+      <Value>620</Value>
+      <Value>619</Value>
+      <Value>219</Value>
+      <Value>536</Value>
+    </TaxCatchAll>
+    <a707137999d24c5390df78a72943486a xmlns="99b93dda-0db1-4804-bcd9-79ac3408f7b3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Stasjonsnett og prøvetakere</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">dd0207a7-2d0a-4417-838c-fdce6848318b</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Kalking</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6d74b546-8f21-4782-aa30-c3b6c259d9bc</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Vannkjemikontrollen</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8379c43c-5bcc-430c-8c15-d982cef44326</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Avtale 2016</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">426aae43-8bc2-4ddf-b2c6-6c511db79aef</TermId>
+        </TermInfo>
+      </Terms>
+    </a707137999d24c5390df78a72943486a>
+    <AvtaltDato xmlns="99b93dda-0db1-4804-bcd9-79ac3408f7b3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Miljødirektoratet Dokument" ma:contentTypeID="0x010100D14BD004BF1C4459B890F3727F0925800030788E1E5F06E4499248722442C9E1E2" ma:contentTypeVersion="4" ma:contentTypeDescription="Opprett et nytt dokument. " ma:contentTypeScope="" ma:versionID="31d2f06e1319184035b49374dedadd14">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99b93dda-0db1-4804-bcd9-79ac3408f7b3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b39a69652e56cca026e8bfba402999b" ns2:_="">
     <xsd:import namespace="99b93dda-0db1-4804-bcd9-79ac3408f7b3"/>
@@ -25869,61 +25952,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <gdc15e87e6184dc285cecc59dfe3e409 xmlns="99b93dda-0db1-4804-bcd9-79ac3408f7b3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </gdc15e87e6184dc285cecc59dfe3e409>
-    <TaxCatchAll xmlns="99b93dda-0db1-4804-bcd9-79ac3408f7b3">
-      <Value>620</Value>
-      <Value>619</Value>
-      <Value>219</Value>
-      <Value>536</Value>
-    </TaxCatchAll>
-    <a707137999d24c5390df78a72943486a xmlns="99b93dda-0db1-4804-bcd9-79ac3408f7b3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Stasjonsnett og prøvetakere</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">dd0207a7-2d0a-4417-838c-fdce6848318b</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Kalking</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6d74b546-8f21-4782-aa30-c3b6c259d9bc</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Vannkjemikontrollen</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8379c43c-5bcc-430c-8c15-d982cef44326</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Avtale 2016</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">426aae43-8bc2-4ddf-b2c6-6c511db79aef</TermId>
-        </TermInfo>
-      </Terms>
-    </a707137999d24c5390df78a72943486a>
-    <AvtaltDato xmlns="99b93dda-0db1-4804-bcd9-79ac3408f7b3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="f3010fb3-0ead-40f9-8418-3186255a05f9" ContentTypeId="0x010100D14BD004BF1C4459B890F3727F092580" PreviousValue="false"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{045B6229-1055-4164-AB1C-6A3398378E43}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E2C70A-39DB-4E9F-AC55-CF83C6FAF41A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="99b93dda-0db1-4804-bcd9-79ac3408f7b3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3C45CF2-DB67-4850-A387-8CB1B8396D69}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{465F94C6-DADA-41F7-9419-4CB4FA36834F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25941,26 +25999,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3C45CF2-DB67-4850-A387-8CB1B8396D69}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{045B6229-1055-4164-AB1C-6A3398378E43}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E2C70A-39DB-4E9F-AC55-CF83C6FAF41A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="99b93dda-0db1-4804-bcd9-79ac3408f7b3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix error in station codes
</commit_message>
<xml_diff>
--- a/data/active_stations_2020.xlsx
+++ b/data/active_stations_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Oeyvind_G\Tiltaksovervakingen\tiltaksovervakingen\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430D2288-6319-4329-9BC3-A652DA83F69F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1C2D69-BF03-4329-82D4-FD46A2500E7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1480,9 +1480,6 @@
     <t>027-58833</t>
   </si>
   <si>
-    <t>027-47427</t>
-  </si>
-  <si>
     <t>027-58831</t>
   </si>
   <si>
@@ -1561,9 +1558,6 @@
     <t>030-58835</t>
   </si>
   <si>
-    <t>030-58776</t>
-  </si>
-  <si>
     <t>030-47471</t>
   </si>
   <si>
@@ -2093,6 +2087,12 @@
   </si>
   <si>
     <t xml:space="preserve">Ny stasjon juli 2020. Prøvetas nedstrøms Kattefossen, ved Røyknesvegen. </t>
+  </si>
+  <si>
+    <t>027-59614</t>
+  </si>
+  <si>
+    <t>030-30839</t>
   </si>
 </sst>
 </file>
@@ -2199,8 +2199,8 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>804863</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>100013</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2216,7 +2216,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="166688" y="152400"/>
-          <a:ext cx="7191375" cy="1214438"/>
+          <a:ext cx="7191375" cy="5105400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2262,6 +2262,19 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
             <a:t>K:\Prosjekter\langtransporterte forurensninger\Kalk Tiltaksovervåking\12 KS vannkjemi\Vannlokaliteter koordinater_kun aktive stasj 2020.xlsx</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>Update 16.08.2021: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Corrected station codes for "Utløp Ørsdalsvatn" and "Espedalselva ved Helle" (see e-mail from Kjetil received 27.05.2021 at 17:15 for details).</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -19008,9 +19021,9 @@
   <dimension ref="A1:K219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="C198" sqref="C198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -19030,37 +19043,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
+        <v>663</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>664</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>665</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>666</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>670</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>671</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>672</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>673</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>667</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>668</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>671</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>672</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>673</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>674</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>675</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>669</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
@@ -19074,7 +19087,7 @@
         <v>454</v>
       </c>
       <c r="E2" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="G2" s="7">
         <v>292044.86731100001</v>
@@ -19086,7 +19099,7 @@
         <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
@@ -19118,7 +19131,7 @@
         <v>33</v>
       </c>
       <c r="J3" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K3" t="s">
         <v>44</v>
@@ -19150,7 +19163,7 @@
         <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K4" t="s">
         <v>400</v>
@@ -19182,7 +19195,7 @@
         <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
@@ -19211,7 +19224,7 @@
         <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K6" t="s">
         <v>457</v>
@@ -19246,7 +19259,7 @@
         <v>33</v>
       </c>
       <c r="J7" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
@@ -19275,7 +19288,7 @@
         <v>33</v>
       </c>
       <c r="J8" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
@@ -19304,7 +19317,7 @@
         <v>33</v>
       </c>
       <c r="J9" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
@@ -19333,7 +19346,7 @@
         <v>33</v>
       </c>
       <c r="J10" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K10" t="s">
         <v>7</v>
@@ -19365,7 +19378,7 @@
         <v>33</v>
       </c>
       <c r="J11" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K11" t="s">
         <v>3</v>
@@ -19397,7 +19410,7 @@
         <v>33</v>
       </c>
       <c r="J12" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K12" t="s">
         <v>5</v>
@@ -19429,7 +19442,7 @@
         <v>33</v>
       </c>
       <c r="J13" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
@@ -19458,7 +19471,7 @@
         <v>33</v>
       </c>
       <c r="J14" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
@@ -19472,7 +19485,7 @@
         <v>391</v>
       </c>
       <c r="E15" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="G15" s="7">
         <v>131566</v>
@@ -19484,7 +19497,7 @@
         <v>33</v>
       </c>
       <c r="J15" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K15" t="s">
         <v>419</v>
@@ -19516,7 +19529,7 @@
         <v>33</v>
       </c>
       <c r="J16" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K16" t="s">
         <v>341</v>
@@ -19533,7 +19546,7 @@
         <v>455</v>
       </c>
       <c r="E17" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="G17" s="7">
         <v>109017.94520099999</v>
@@ -19545,7 +19558,7 @@
         <v>33</v>
       </c>
       <c r="J17" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K17" t="s">
         <v>398</v>
@@ -19562,7 +19575,7 @@
         <v>456</v>
       </c>
       <c r="E18" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="G18" s="7">
         <v>108864.263483</v>
@@ -19574,7 +19587,7 @@
         <v>33</v>
       </c>
       <c r="J18" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K18" t="s">
         <v>398</v>
@@ -19606,7 +19619,7 @@
         <v>33</v>
       </c>
       <c r="J19" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
@@ -19635,7 +19648,7 @@
         <v>33</v>
       </c>
       <c r="J20" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.45">
@@ -19664,7 +19677,7 @@
         <v>33</v>
       </c>
       <c r="J21" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.45">
@@ -19693,7 +19706,7 @@
         <v>33</v>
       </c>
       <c r="J22" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
@@ -19725,7 +19738,7 @@
         <v>33</v>
       </c>
       <c r="J23" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K23" t="s">
         <v>30</v>
@@ -19757,7 +19770,7 @@
         <v>33</v>
       </c>
       <c r="J24" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.45">
@@ -19789,7 +19802,7 @@
         <v>33</v>
       </c>
       <c r="J25" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.45">
@@ -19815,7 +19828,7 @@
         <v>33</v>
       </c>
       <c r="J26" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K26" t="s">
         <v>342</v>
@@ -19832,7 +19845,7 @@
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="E27" t="s">
         <v>415</v>
@@ -19847,7 +19860,7 @@
         <v>33</v>
       </c>
       <c r="J27" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K27" t="s">
         <v>26</v>
@@ -19879,7 +19892,7 @@
         <v>33</v>
       </c>
       <c r="J28" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="K28" t="s">
         <v>383</v>
@@ -19911,7 +19924,7 @@
         <v>33</v>
       </c>
       <c r="J29" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="K29" t="s">
         <v>381</v>
@@ -19925,10 +19938,10 @@
         <v>330</v>
       </c>
       <c r="C30" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E30" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="G30" s="7">
         <v>83862</v>
@@ -19940,10 +19953,10 @@
         <v>33</v>
       </c>
       <c r="J30" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K30" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.45">
@@ -19969,7 +19982,7 @@
         <v>33</v>
       </c>
       <c r="J31" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="K31" t="s">
         <v>382</v>
@@ -19998,7 +20011,7 @@
         <v>33</v>
       </c>
       <c r="J32" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K32" t="s">
         <v>420</v>
@@ -20027,7 +20040,7 @@
         <v>33</v>
       </c>
       <c r="J33" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K33" t="s">
         <v>420</v>
@@ -20056,7 +20069,7 @@
         <v>33</v>
       </c>
       <c r="J34" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K34" t="s">
         <v>385</v>
@@ -20088,7 +20101,7 @@
         <v>33</v>
       </c>
       <c r="J35" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K35" t="s">
         <v>384</v>
@@ -20120,7 +20133,7 @@
         <v>33</v>
       </c>
       <c r="J36" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K36" t="s">
         <v>384</v>
@@ -20134,10 +20147,10 @@
         <v>330</v>
       </c>
       <c r="C37" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E37" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="G37" s="8">
         <v>85526</v>
@@ -20149,10 +20162,10 @@
         <v>33</v>
       </c>
       <c r="J37" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="K37" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.45">
@@ -20163,10 +20176,10 @@
         <v>330</v>
       </c>
       <c r="C38" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="E38" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="G38" s="8">
         <v>83953</v>
@@ -20178,10 +20191,10 @@
         <v>33</v>
       </c>
       <c r="J38" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K38" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.45">
@@ -20207,7 +20220,7 @@
         <v>33</v>
       </c>
       <c r="J39" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K39" t="s">
         <v>420</v>
@@ -20236,7 +20249,7 @@
         <v>33</v>
       </c>
       <c r="J40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K40" t="s">
         <v>50</v>
@@ -20253,7 +20266,7 @@
         <v>52</v>
       </c>
       <c r="E41" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="G41" s="7">
         <v>71614</v>
@@ -20265,7 +20278,7 @@
         <v>33</v>
       </c>
       <c r="J41" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K41" t="s">
         <v>343</v>
@@ -20294,7 +20307,7 @@
         <v>33</v>
       </c>
       <c r="J42" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K42" t="s">
         <v>343</v>
@@ -20323,7 +20336,7 @@
         <v>33</v>
       </c>
       <c r="J43" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K43" t="s">
         <v>343</v>
@@ -20340,7 +20353,7 @@
         <v>321</v>
       </c>
       <c r="E44" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="G44" s="7">
         <v>78337.500564999995</v>
@@ -20352,7 +20365,7 @@
         <v>33</v>
       </c>
       <c r="J44" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.45">
@@ -20381,7 +20394,7 @@
         <v>33</v>
       </c>
       <c r="J45" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K45" t="s">
         <v>323</v>
@@ -20413,7 +20426,7 @@
         <v>33</v>
       </c>
       <c r="J46" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K46" t="s">
         <v>323</v>
@@ -20445,7 +20458,7 @@
         <v>33</v>
       </c>
       <c r="J47" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K47" t="s">
         <v>323</v>
@@ -20477,7 +20490,7 @@
         <v>33</v>
       </c>
       <c r="J48" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.45">
@@ -20506,7 +20519,7 @@
         <v>33</v>
       </c>
       <c r="J49" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.45">
@@ -20535,7 +20548,7 @@
         <v>33</v>
       </c>
       <c r="J50" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.45">
@@ -20561,7 +20574,7 @@
         <v>33</v>
       </c>
       <c r="J51" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K51" t="s">
         <v>376</v>
@@ -20593,7 +20606,7 @@
         <v>33</v>
       </c>
       <c r="J52" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.45">
@@ -20622,7 +20635,7 @@
         <v>33</v>
       </c>
       <c r="J53" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.45">
@@ -20651,7 +20664,7 @@
         <v>33</v>
       </c>
       <c r="J54" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.45">
@@ -20677,7 +20690,7 @@
         <v>33</v>
       </c>
       <c r="J55" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K55" t="s">
         <v>377</v>
@@ -20706,7 +20719,7 @@
         <v>33</v>
       </c>
       <c r="J56" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="K56" t="s">
         <v>378</v>
@@ -20741,7 +20754,7 @@
         <v>33</v>
       </c>
       <c r="J57" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.45">
@@ -20773,7 +20786,7 @@
         <v>33</v>
       </c>
       <c r="J58" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.45">
@@ -20802,7 +20815,7 @@
         <v>33</v>
       </c>
       <c r="J59" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.45">
@@ -20831,7 +20844,7 @@
         <v>33</v>
       </c>
       <c r="J60" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.45">
@@ -20845,7 +20858,7 @@
         <v>281</v>
       </c>
       <c r="D61" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E61" t="s">
         <v>431</v>
@@ -20860,7 +20873,7 @@
         <v>33</v>
       </c>
       <c r="J61" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.45">
@@ -20889,7 +20902,7 @@
         <v>33</v>
       </c>
       <c r="J62" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.45">
@@ -20903,7 +20916,7 @@
         <v>278</v>
       </c>
       <c r="D63" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="E63" t="s">
         <v>433</v>
@@ -20918,7 +20931,7 @@
         <v>33</v>
       </c>
       <c r="J63" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="K63" t="s">
         <v>373</v>
@@ -20935,7 +20948,7 @@
         <v>279</v>
       </c>
       <c r="D64" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E64" t="s">
         <v>434</v>
@@ -20950,7 +20963,7 @@
         <v>33</v>
       </c>
       <c r="J64" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="K64" t="s">
         <v>374</v>
@@ -20982,7 +20995,7 @@
         <v>33</v>
       </c>
       <c r="J65" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.45">
@@ -21011,7 +21024,7 @@
         <v>33</v>
       </c>
       <c r="J66" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K66" t="s">
         <v>283</v>
@@ -21043,7 +21056,7 @@
         <v>33</v>
       </c>
       <c r="J67" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.45">
@@ -21072,7 +21085,7 @@
         <v>33</v>
       </c>
       <c r="J68" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.45">
@@ -21101,7 +21114,7 @@
         <v>33</v>
       </c>
       <c r="J69" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.45">
@@ -21130,7 +21143,7 @@
         <v>33</v>
       </c>
       <c r="J70" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.45">
@@ -21156,7 +21169,7 @@
         <v>33</v>
       </c>
       <c r="J71" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K71" t="s">
         <v>386</v>
@@ -21173,7 +21186,7 @@
         <v>395</v>
       </c>
       <c r="E72" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="G72" s="7">
         <v>33005</v>
@@ -21185,7 +21198,7 @@
         <v>33</v>
       </c>
       <c r="J72" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K72" t="s">
         <v>436</v>
@@ -21217,7 +21230,7 @@
         <v>33</v>
       </c>
       <c r="J73" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.45">
@@ -21246,7 +21259,7 @@
         <v>33</v>
       </c>
       <c r="J74" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.45">
@@ -21275,7 +21288,7 @@
         <v>33</v>
       </c>
       <c r="J75" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.45">
@@ -21304,7 +21317,7 @@
         <v>33</v>
       </c>
       <c r="J76" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.45">
@@ -21318,7 +21331,7 @@
         <v>291</v>
       </c>
       <c r="D77" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E77" t="s">
         <v>447</v>
@@ -21333,7 +21346,7 @@
         <v>33</v>
       </c>
       <c r="J77" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.45">
@@ -21362,7 +21375,7 @@
         <v>33</v>
       </c>
       <c r="J78" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.45">
@@ -21391,7 +21404,7 @@
         <v>33</v>
       </c>
       <c r="J79" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.45">
@@ -21420,7 +21433,7 @@
         <v>33</v>
       </c>
       <c r="J80" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K80" t="s">
         <v>375</v>
@@ -21449,7 +21462,7 @@
         <v>33</v>
       </c>
       <c r="J81" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.45">
@@ -21478,7 +21491,7 @@
         <v>33</v>
       </c>
       <c r="J82" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K82" t="s">
         <v>317</v>
@@ -21510,7 +21523,7 @@
         <v>33</v>
       </c>
       <c r="J83" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.45">
@@ -21539,7 +21552,7 @@
         <v>33</v>
       </c>
       <c r="J84" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K84" t="s">
         <v>380</v>
@@ -21568,7 +21581,7 @@
         <v>33</v>
       </c>
       <c r="J85" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K85" t="s">
         <v>379</v>
@@ -21600,7 +21613,7 @@
         <v>33</v>
       </c>
       <c r="J86" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K86" t="s">
         <v>467</v>
@@ -21616,8 +21629,11 @@
       <c r="C87" t="s">
         <v>396</v>
       </c>
+      <c r="D87">
+        <v>6</v>
+      </c>
       <c r="E87" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="G87" s="7">
         <v>344012</v>
@@ -21629,7 +21645,7 @@
         <v>32</v>
       </c>
       <c r="J87" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K87" t="s">
         <v>437</v>
@@ -21661,7 +21677,7 @@
         <v>33</v>
       </c>
       <c r="J88" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.45">
@@ -21690,7 +21706,7 @@
         <v>33</v>
       </c>
       <c r="J89" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.45">
@@ -21719,7 +21735,7 @@
         <v>33</v>
       </c>
       <c r="J90" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.45">
@@ -21748,7 +21764,7 @@
         <v>33</v>
       </c>
       <c r="J91" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.45">
@@ -21774,7 +21790,7 @@
         <v>33</v>
       </c>
       <c r="J92" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K92" t="s">
         <v>363</v>
@@ -21803,7 +21819,7 @@
         <v>33</v>
       </c>
       <c r="J93" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K93" t="s">
         <v>363</v>
@@ -21835,7 +21851,7 @@
         <v>33</v>
       </c>
       <c r="J94" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K94" t="s">
         <v>364</v>
@@ -21864,7 +21880,7 @@
         <v>33</v>
       </c>
       <c r="J95" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K95" t="s">
         <v>363</v>
@@ -21893,7 +21909,7 @@
         <v>33</v>
       </c>
       <c r="J96" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K96" t="s">
         <v>363</v>
@@ -21925,7 +21941,7 @@
         <v>33</v>
       </c>
       <c r="J97" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K97" t="s">
         <v>365</v>
@@ -21957,7 +21973,7 @@
         <v>33</v>
       </c>
       <c r="J98" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.45">
@@ -21986,7 +22002,7 @@
         <v>33</v>
       </c>
       <c r="J99" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.45">
@@ -22015,7 +22031,7 @@
         <v>33</v>
       </c>
       <c r="J100" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.45">
@@ -22044,7 +22060,7 @@
         <v>33</v>
       </c>
       <c r="J101" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.45">
@@ -22073,7 +22089,7 @@
         <v>33</v>
       </c>
       <c r="J102" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.45">
@@ -22102,7 +22118,7 @@
         <v>33</v>
       </c>
       <c r="J103" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.45">
@@ -22119,7 +22135,7 @@
         <v>12</v>
       </c>
       <c r="E104" t="s">
-        <v>482</v>
+        <v>685</v>
       </c>
       <c r="G104" s="7">
         <v>-15325.023718</v>
@@ -22131,7 +22147,7 @@
         <v>33</v>
       </c>
       <c r="J104" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.45">
@@ -22148,7 +22164,7 @@
         <v>14</v>
       </c>
       <c r="E105" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G105" s="7">
         <v>-9237.6714699999993</v>
@@ -22160,7 +22176,7 @@
         <v>33</v>
       </c>
       <c r="J105" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K105" t="s">
         <v>147</v>
@@ -22180,7 +22196,7 @@
         <v>15</v>
       </c>
       <c r="E106" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G106" s="7">
         <v>-9693.6067800000001</v>
@@ -22192,7 +22208,7 @@
         <v>33</v>
       </c>
       <c r="J106" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K106" t="s">
         <v>145</v>
@@ -22206,13 +22222,13 @@
         <v>175</v>
       </c>
       <c r="C107" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D107">
         <v>4</v>
       </c>
       <c r="E107" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G107" s="7">
         <v>-32671.270689000001</v>
@@ -22224,10 +22240,10 @@
         <v>33</v>
       </c>
       <c r="J107" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K107" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.45">
@@ -22244,7 +22260,7 @@
         <v>48</v>
       </c>
       <c r="E108" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G108" s="7">
         <v>-21333.146041</v>
@@ -22256,10 +22272,10 @@
         <v>33</v>
       </c>
       <c r="J108" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K108" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.45">
@@ -22276,7 +22292,7 @@
         <v>50</v>
       </c>
       <c r="E109" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G109" s="7">
         <v>-23756.366348</v>
@@ -22288,7 +22304,7 @@
         <v>33</v>
       </c>
       <c r="J109" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.45">
@@ -22305,7 +22321,7 @@
         <v>51</v>
       </c>
       <c r="E110" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G110" s="7">
         <v>-23746.894015999998</v>
@@ -22317,7 +22333,7 @@
         <v>33</v>
       </c>
       <c r="J110" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.45">
@@ -22334,7 +22350,7 @@
         <v>52</v>
       </c>
       <c r="E111" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G111" s="7">
         <v>-32698.885877000001</v>
@@ -22346,10 +22362,10 @@
         <v>33</v>
       </c>
       <c r="J111" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K111" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.45">
@@ -22360,7 +22376,7 @@
         <v>175</v>
       </c>
       <c r="C112" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D112">
         <v>53</v>
@@ -22381,10 +22397,10 @@
         <v>33</v>
       </c>
       <c r="J112" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K112" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.45">
@@ -22401,7 +22417,7 @@
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G113" s="7">
         <v>-967.01564800000006</v>
@@ -22413,7 +22429,7 @@
         <v>33</v>
       </c>
       <c r="J113" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K113" t="s">
         <v>166</v>
@@ -22427,16 +22443,16 @@
         <v>159</v>
       </c>
       <c r="C114" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D114">
         <v>2</v>
       </c>
       <c r="E114" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F114" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G114" s="7">
         <v>2426.211605</v>
@@ -22448,7 +22464,7 @@
         <v>33</v>
       </c>
       <c r="J114" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K114" t="s">
         <v>160</v>
@@ -22483,7 +22499,7 @@
         <v>33</v>
       </c>
       <c r="J115" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K115" t="s">
         <v>162</v>
@@ -22497,16 +22513,16 @@
         <v>159</v>
       </c>
       <c r="C116" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D116">
         <v>4</v>
       </c>
       <c r="E116" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F116" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G116" s="7">
         <v>2589.447658</v>
@@ -22518,7 +22534,7 @@
         <v>33</v>
       </c>
       <c r="J116" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K116" t="s">
         <v>356</v>
@@ -22532,16 +22548,16 @@
         <v>159</v>
       </c>
       <c r="C117" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D117">
         <v>5</v>
       </c>
       <c r="E117" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F117" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G117" s="7">
         <v>3231.5613589999998</v>
@@ -22553,7 +22569,7 @@
         <v>33</v>
       </c>
       <c r="J117" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="K117" t="s">
         <v>357</v>
@@ -22570,10 +22586,10 @@
         <v>158</v>
       </c>
       <c r="D118" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E118" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G118" s="7">
         <v>-435.61006500000002</v>
@@ -22585,7 +22601,7 @@
         <v>33</v>
       </c>
       <c r="J118" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.45">
@@ -22602,7 +22618,7 @@
         <v>1</v>
       </c>
       <c r="E119" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G119" s="7">
         <v>-445.99656299999998</v>
@@ -22614,7 +22630,7 @@
         <v>33</v>
       </c>
       <c r="J119" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K119" t="s">
         <v>157</v>
@@ -22634,7 +22650,7 @@
         <v>3</v>
       </c>
       <c r="E120" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G120" s="7">
         <v>-4131.4289749999998</v>
@@ -22646,7 +22662,7 @@
         <v>33</v>
       </c>
       <c r="J120" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.45">
@@ -22663,7 +22679,7 @@
         <v>5</v>
       </c>
       <c r="E121" t="s">
-        <v>509</v>
+        <v>686</v>
       </c>
       <c r="G121" s="7">
         <v>-9405.6402849999995</v>
@@ -22675,7 +22691,7 @@
         <v>33</v>
       </c>
       <c r="J121" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.45">
@@ -22692,7 +22708,7 @@
         <v>6</v>
       </c>
       <c r="E122" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="G122" s="7">
         <v>847.46973000000003</v>
@@ -22704,7 +22720,7 @@
         <v>33</v>
       </c>
       <c r="J122" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.45">
@@ -22715,13 +22731,13 @@
         <v>172</v>
       </c>
       <c r="C123" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D123">
         <v>1</v>
       </c>
       <c r="E123" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G123" s="7">
         <v>24767.383523</v>
@@ -22733,7 +22749,7 @@
         <v>33</v>
       </c>
       <c r="J123" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.45">
@@ -22744,13 +22760,13 @@
         <v>172</v>
       </c>
       <c r="C124" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D124">
         <v>3</v>
       </c>
       <c r="E124" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="G124" s="7">
         <v>22269.240881000002</v>
@@ -22762,7 +22778,7 @@
         <v>33</v>
       </c>
       <c r="J124" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.45">
@@ -22773,13 +22789,13 @@
         <v>172</v>
       </c>
       <c r="C125" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D125">
         <v>4</v>
       </c>
       <c r="E125" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="G125" s="7">
         <v>22042.742042999998</v>
@@ -22791,7 +22807,7 @@
         <v>33</v>
       </c>
       <c r="J125" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K125" t="s">
         <v>174</v>
@@ -22811,7 +22827,7 @@
         <v>7</v>
       </c>
       <c r="E126" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="G126" s="7">
         <v>23098.613496999998</v>
@@ -22823,7 +22839,7 @@
         <v>33</v>
       </c>
       <c r="J126" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.45">
@@ -22837,7 +22853,7 @@
         <v>168</v>
       </c>
       <c r="D127" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="E127" t="s">
         <v>169</v>
@@ -22855,10 +22871,10 @@
         <v>33</v>
       </c>
       <c r="J127" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K127" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.45">
@@ -22875,7 +22891,7 @@
         <v>4</v>
       </c>
       <c r="E128" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="G128" s="7">
         <v>-13128.407453</v>
@@ -22887,7 +22903,7 @@
         <v>33</v>
       </c>
       <c r="J128" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.45">
@@ -22898,7 +22914,7 @@
         <v>206</v>
       </c>
       <c r="C129" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D129">
         <v>11</v>
@@ -22916,7 +22932,7 @@
         <v>33</v>
       </c>
       <c r="J129" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.45">
@@ -22927,7 +22943,7 @@
         <v>206</v>
       </c>
       <c r="C130" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D130">
         <v>12</v>
@@ -22945,7 +22961,7 @@
         <v>33</v>
       </c>
       <c r="J130" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K130" t="s">
         <v>366</v>
@@ -22977,7 +22993,7 @@
         <v>33</v>
       </c>
       <c r="J131" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.45">
@@ -22988,7 +23004,7 @@
         <v>206</v>
       </c>
       <c r="C132" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D132">
         <v>14</v>
@@ -23006,7 +23022,7 @@
         <v>33</v>
       </c>
       <c r="J132" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.45">
@@ -23035,7 +23051,7 @@
         <v>33</v>
       </c>
       <c r="J133" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.45">
@@ -23064,7 +23080,7 @@
         <v>33</v>
       </c>
       <c r="J134" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K134" t="s">
         <v>367</v>
@@ -23081,7 +23097,7 @@
         <v>224</v>
       </c>
       <c r="D135" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E135" t="s">
         <v>225</v>
@@ -23096,7 +23112,7 @@
         <v>33</v>
       </c>
       <c r="J135" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.45">
@@ -23110,7 +23126,7 @@
         <v>222</v>
       </c>
       <c r="D136" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E136" t="s">
         <v>223</v>
@@ -23125,7 +23141,7 @@
         <v>33</v>
       </c>
       <c r="J136" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.45">
@@ -23139,7 +23155,7 @@
         <v>218</v>
       </c>
       <c r="D137" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="E137" t="s">
         <v>219</v>
@@ -23154,7 +23170,7 @@
         <v>33</v>
       </c>
       <c r="J137" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.45">
@@ -23168,7 +23184,7 @@
         <v>216</v>
       </c>
       <c r="D138" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E138" t="s">
         <v>217</v>
@@ -23183,7 +23199,7 @@
         <v>33</v>
       </c>
       <c r="J138" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.45">
@@ -23197,7 +23213,7 @@
         <v>207</v>
       </c>
       <c r="D139" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E139" t="s">
         <v>208</v>
@@ -23212,7 +23228,7 @@
         <v>33</v>
       </c>
       <c r="J139" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.45">
@@ -23223,10 +23239,10 @@
         <v>206</v>
       </c>
       <c r="C140" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D140" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E140" t="s">
         <v>226</v>
@@ -23241,7 +23257,7 @@
         <v>33</v>
       </c>
       <c r="J140" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K140" t="s">
         <v>368</v>
@@ -23255,10 +23271,10 @@
         <v>206</v>
       </c>
       <c r="C141" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D141" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E141" t="s">
         <v>227</v>
@@ -23273,7 +23289,7 @@
         <v>33</v>
       </c>
       <c r="J141" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K141" t="s">
         <v>369</v>
@@ -23287,10 +23303,10 @@
         <v>206</v>
       </c>
       <c r="C142" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D142" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E142" t="s">
         <v>228</v>
@@ -23305,7 +23321,7 @@
         <v>33</v>
       </c>
       <c r="J142" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K142" t="s">
         <v>247</v>
@@ -23322,10 +23338,10 @@
         <v>236</v>
       </c>
       <c r="D143" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E143" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="G143" s="7">
         <v>-13388.353966000001</v>
@@ -23337,7 +23353,7 @@
         <v>33</v>
       </c>
       <c r="J143" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.45">
@@ -23351,7 +23367,7 @@
         <v>233</v>
       </c>
       <c r="D144" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="E144" t="s">
         <v>234</v>
@@ -23369,10 +23385,10 @@
         <v>32</v>
       </c>
       <c r="J144" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K144" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.45">
@@ -23386,10 +23402,10 @@
         <v>232</v>
       </c>
       <c r="D145" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="E145" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="G145" s="7">
         <v>-10380.171338</v>
@@ -23401,7 +23417,7 @@
         <v>33</v>
       </c>
       <c r="J145" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.45">
@@ -23415,10 +23431,10 @@
         <v>231</v>
       </c>
       <c r="D146" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="E146" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="G146" s="7">
         <v>-9248.3661780000002</v>
@@ -23430,7 +23446,7 @@
         <v>33</v>
       </c>
       <c r="J146" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.45">
@@ -23444,10 +23460,10 @@
         <v>230</v>
       </c>
       <c r="D147" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="E147" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="G147" s="7">
         <v>-9339.310442</v>
@@ -23459,7 +23475,7 @@
         <v>33</v>
       </c>
       <c r="J147" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.45">
@@ -23470,10 +23486,10 @@
         <v>229</v>
       </c>
       <c r="C148" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D148" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="E148" t="s">
         <v>237</v>
@@ -23488,7 +23504,7 @@
         <v>33</v>
       </c>
       <c r="J148" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K148" t="s">
         <v>370</v>
@@ -23505,7 +23521,7 @@
         <v>360</v>
       </c>
       <c r="D149" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E149" t="s">
         <v>186</v>
@@ -23523,7 +23539,7 @@
         <v>33</v>
       </c>
       <c r="J149" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K149" t="s">
         <v>361</v>
@@ -23540,7 +23556,7 @@
         <v>188</v>
       </c>
       <c r="D150" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="E150" t="s">
         <v>189</v>
@@ -23555,7 +23571,7 @@
         <v>33</v>
       </c>
       <c r="J150" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K150" t="s">
         <v>362</v>
@@ -23572,7 +23588,7 @@
         <v>359</v>
       </c>
       <c r="D151" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="E151" t="s">
         <v>185</v>
@@ -23587,7 +23603,7 @@
         <v>33</v>
       </c>
       <c r="J151" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K151" t="s">
         <v>358</v>
@@ -23604,13 +23620,13 @@
         <v>183</v>
       </c>
       <c r="D152" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="E152" t="s">
         <v>184</v>
       </c>
       <c r="F152" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="G152" s="7">
         <v>-15236</v>
@@ -23622,10 +23638,10 @@
         <v>33</v>
       </c>
       <c r="J152" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K152" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.45">
@@ -23636,16 +23652,16 @@
         <v>93</v>
       </c>
       <c r="C153" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D153" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E153" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F153" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="G153" s="7">
         <v>-9606.8189999999995</v>
@@ -23657,7 +23673,7 @@
         <v>33</v>
       </c>
       <c r="J153" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.45">
@@ -23668,16 +23684,16 @@
         <v>93</v>
       </c>
       <c r="C154" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D154" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E154" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F154" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="G154" s="7">
         <v>-7081.4575999999997</v>
@@ -23689,7 +23705,7 @@
         <v>33</v>
       </c>
       <c r="J154" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.45">
@@ -23700,16 +23716,16 @@
         <v>93</v>
       </c>
       <c r="C155" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D155" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E155" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="F155" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="G155" s="7">
         <v>-7682.8486999999996</v>
@@ -23721,10 +23737,10 @@
         <v>33</v>
       </c>
       <c r="J155" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K155" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.45">
@@ -23735,16 +23751,16 @@
         <v>93</v>
       </c>
       <c r="C156" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D156" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="E156" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="F156" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="G156" s="7">
         <v>-7941.6787000000004</v>
@@ -23756,10 +23772,10 @@
         <v>33</v>
       </c>
       <c r="J156" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K156" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.45">
@@ -23773,7 +23789,7 @@
         <v>89</v>
       </c>
       <c r="E157" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="G157" s="7">
         <v>-1511.7375999999999</v>
@@ -23785,7 +23801,7 @@
         <v>33</v>
       </c>
       <c r="J157" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.45">
@@ -23799,7 +23815,7 @@
         <v>88</v>
       </c>
       <c r="E158" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="G158" s="7">
         <v>205.46729999999999</v>
@@ -23811,7 +23827,7 @@
         <v>33</v>
       </c>
       <c r="J158" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.45">
@@ -23825,10 +23841,10 @@
         <v>90</v>
       </c>
       <c r="D159" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E159" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="G159" s="7">
         <v>-5621.3424999999997</v>
@@ -23840,7 +23856,7 @@
         <v>33</v>
       </c>
       <c r="J159" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.45">
@@ -23854,10 +23870,10 @@
         <v>91</v>
       </c>
       <c r="D160" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E160" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="G160" s="7">
         <v>-5808.415</v>
@@ -23869,7 +23885,7 @@
         <v>33</v>
       </c>
       <c r="J160" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K160" t="s">
         <v>344</v>
@@ -23886,10 +23902,10 @@
         <v>92</v>
       </c>
       <c r="D161" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="E161" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="G161" s="7">
         <v>-7743.46</v>
@@ -23901,7 +23917,7 @@
         <v>33</v>
       </c>
       <c r="J161" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.45">
@@ -23915,10 +23931,10 @@
         <v>60</v>
       </c>
       <c r="D162" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E162" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="G162" s="7">
         <v>-1325.5878</v>
@@ -23930,7 +23946,7 @@
         <v>33</v>
       </c>
       <c r="J162" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.45">
@@ -23944,10 +23960,10 @@
         <v>61</v>
       </c>
       <c r="D163" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E163" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="G163" s="7">
         <v>-2308.2676999999999</v>
@@ -23959,7 +23975,7 @@
         <v>33</v>
       </c>
       <c r="J163" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.45">
@@ -23973,10 +23989,10 @@
         <v>97</v>
       </c>
       <c r="D164" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E164" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="G164" s="7">
         <v>37414.972500000003</v>
@@ -23988,7 +24004,7 @@
         <v>33</v>
       </c>
       <c r="J164" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.45">
@@ -24002,10 +24018,10 @@
         <v>98</v>
       </c>
       <c r="D165" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="G165" s="7">
         <v>32589.801899999999</v>
@@ -24017,7 +24033,7 @@
         <v>33</v>
       </c>
       <c r="J165" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.45">
@@ -24031,10 +24047,10 @@
         <v>96</v>
       </c>
       <c r="D166" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="E166" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="G166" s="7">
         <v>17092.468199999999</v>
@@ -24046,7 +24062,7 @@
         <v>33</v>
       </c>
       <c r="J166" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.45">
@@ -24060,10 +24076,10 @@
         <v>99</v>
       </c>
       <c r="D167" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E167" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="G167" s="7">
         <v>14021.164199999999</v>
@@ -24075,7 +24091,7 @@
         <v>33</v>
       </c>
       <c r="J167" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.45">
@@ -24089,10 +24105,10 @@
         <v>95</v>
       </c>
       <c r="D168" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="E168" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="G168" s="7">
         <v>6492.1962000000003</v>
@@ -24104,7 +24120,7 @@
         <v>33</v>
       </c>
       <c r="J168" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.45">
@@ -24118,10 +24134,10 @@
         <v>100</v>
       </c>
       <c r="D169" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="E169" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="G169" s="7">
         <v>14581.5694</v>
@@ -24133,7 +24149,7 @@
         <v>33</v>
       </c>
       <c r="J169" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.45">
@@ -24144,16 +24160,16 @@
         <v>94</v>
       </c>
       <c r="C170" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D170">
         <v>10</v>
       </c>
       <c r="E170" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="F170" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G170" s="7">
         <v>14174.4043</v>
@@ -24165,7 +24181,7 @@
         <v>33</v>
       </c>
       <c r="J170" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.45">
@@ -24179,7 +24195,7 @@
         <v>69</v>
       </c>
       <c r="D171" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E171" t="s">
         <v>70</v>
@@ -24197,7 +24213,7 @@
         <v>33</v>
       </c>
       <c r="J171" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.45">
@@ -24211,7 +24227,7 @@
         <v>81</v>
       </c>
       <c r="D172" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="E172" t="s">
         <v>83</v>
@@ -24229,7 +24245,7 @@
         <v>33</v>
       </c>
       <c r="J172" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K172" t="s">
         <v>82</v>
@@ -24246,7 +24262,7 @@
         <v>75</v>
       </c>
       <c r="D173" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E173" t="s">
         <v>76</v>
@@ -24264,7 +24280,7 @@
         <v>33</v>
       </c>
       <c r="J173" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.45">
@@ -24278,7 +24294,7 @@
         <v>63</v>
       </c>
       <c r="D174" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="E174" t="s">
         <v>64</v>
@@ -24296,7 +24312,7 @@
         <v>33</v>
       </c>
       <c r="J174" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.45">
@@ -24310,7 +24326,7 @@
         <v>66</v>
       </c>
       <c r="D175" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E175" t="s">
         <v>67</v>
@@ -24328,7 +24344,7 @@
         <v>33</v>
       </c>
       <c r="J175" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.45">
@@ -24342,7 +24358,7 @@
         <v>78</v>
       </c>
       <c r="D176" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="E176" t="s">
         <v>79</v>
@@ -24360,7 +24376,7 @@
         <v>33</v>
       </c>
       <c r="J176" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.45">
@@ -24374,7 +24390,7 @@
         <v>85</v>
       </c>
       <c r="D177" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="E177" t="s">
         <v>86</v>
@@ -24392,7 +24408,7 @@
         <v>33</v>
       </c>
       <c r="J177" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.45">
@@ -24406,7 +24422,7 @@
         <v>72</v>
       </c>
       <c r="D178" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="E178" t="s">
         <v>73</v>
@@ -24424,7 +24440,7 @@
         <v>33</v>
       </c>
       <c r="J178" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.45">
@@ -24435,10 +24451,10 @@
         <v>128</v>
       </c>
       <c r="C179" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D179" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E179" t="s">
         <v>129</v>
@@ -24456,7 +24472,7 @@
         <v>33</v>
       </c>
       <c r="J179" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K179" t="s">
         <v>352</v>
@@ -24470,10 +24486,10 @@
         <v>128</v>
       </c>
       <c r="C180" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D180" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E180" t="s">
         <v>132</v>
@@ -24488,7 +24504,7 @@
         <v>33</v>
       </c>
       <c r="J180" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K180" t="s">
         <v>131</v>
@@ -24502,10 +24518,10 @@
         <v>128</v>
       </c>
       <c r="C181" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D181" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="E181" t="s">
         <v>134</v>
@@ -24523,7 +24539,7 @@
         <v>33</v>
       </c>
       <c r="J181" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K181" t="s">
         <v>354</v>
@@ -24537,10 +24553,10 @@
         <v>128</v>
       </c>
       <c r="C182" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D182" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E182" t="s">
         <v>133</v>
@@ -24555,7 +24571,7 @@
         <v>33</v>
       </c>
       <c r="J182" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K182" t="s">
         <v>353</v>
@@ -24569,10 +24585,10 @@
         <v>128</v>
       </c>
       <c r="C183" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D183" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="E183" t="s">
         <v>136</v>
@@ -24587,7 +24603,7 @@
         <v>33</v>
       </c>
       <c r="J183" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K183" t="s">
         <v>131</v>
@@ -24601,10 +24617,10 @@
         <v>128</v>
       </c>
       <c r="C184" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D184" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E184" t="s">
         <v>137</v>
@@ -24622,7 +24638,7 @@
         <v>33</v>
       </c>
       <c r="J184" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K184" t="s">
         <v>355</v>
@@ -24654,7 +24670,7 @@
         <v>33</v>
       </c>
       <c r="J185" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K185" t="s">
         <v>82</v>
@@ -24683,7 +24699,7 @@
         <v>33</v>
       </c>
       <c r="J186" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K186" t="s">
         <v>82</v>
@@ -24715,7 +24731,7 @@
         <v>33</v>
       </c>
       <c r="J187" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K187" t="s">
         <v>82</v>
@@ -24732,7 +24748,7 @@
         <v>106</v>
       </c>
       <c r="D188" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E188" t="s">
         <v>107</v>
@@ -24747,7 +24763,7 @@
         <v>33</v>
       </c>
       <c r="J188" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K188" t="s">
         <v>347</v>
@@ -24764,7 +24780,7 @@
         <v>108</v>
       </c>
       <c r="D189" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E189" t="s">
         <v>109</v>
@@ -24779,7 +24795,7 @@
         <v>33</v>
       </c>
       <c r="J189" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K189" t="s">
         <v>347</v>
@@ -24796,7 +24812,7 @@
         <v>110</v>
       </c>
       <c r="D190" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="E190" t="s">
         <v>111</v>
@@ -24811,7 +24827,7 @@
         <v>33</v>
       </c>
       <c r="J190" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K190" t="s">
         <v>347</v>
@@ -24828,7 +24844,7 @@
         <v>112</v>
       </c>
       <c r="D191" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E191" t="s">
         <v>113</v>
@@ -24843,7 +24859,7 @@
         <v>33</v>
       </c>
       <c r="J191" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K191" t="s">
         <v>347</v>
@@ -24860,7 +24876,7 @@
         <v>115</v>
       </c>
       <c r="D192" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E192" t="s">
         <v>116</v>
@@ -24875,7 +24891,7 @@
         <v>33</v>
       </c>
       <c r="J192" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K192" t="s">
         <v>347</v>
@@ -24892,7 +24908,7 @@
         <v>117</v>
       </c>
       <c r="D193" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E193" t="s">
         <v>118</v>
@@ -24907,7 +24923,7 @@
         <v>33</v>
       </c>
       <c r="J193" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K193" t="s">
         <v>347</v>
@@ -24924,7 +24940,7 @@
         <v>119</v>
       </c>
       <c r="D194" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="E194" t="s">
         <v>120</v>
@@ -24939,7 +24955,7 @@
         <v>33</v>
       </c>
       <c r="J194" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K194" t="s">
         <v>347</v>
@@ -24956,10 +24972,10 @@
         <v>103</v>
       </c>
       <c r="D195" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E195" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G195" s="7">
         <v>-22737.912199999999</v>
@@ -24971,7 +24987,7 @@
         <v>33</v>
       </c>
       <c r="J195" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K195" t="s">
         <v>350</v>
@@ -24988,10 +25004,10 @@
         <v>102</v>
       </c>
       <c r="D196" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E196" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="G196" s="7">
         <v>-27117.159599999999</v>
@@ -25003,7 +25019,7 @@
         <v>33</v>
       </c>
       <c r="J196" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.45">
@@ -25017,10 +25033,10 @@
         <v>101</v>
       </c>
       <c r="D197" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="E197" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="G197" s="7">
         <v>-27524.878000000001</v>
@@ -25032,7 +25048,7 @@
         <v>33</v>
       </c>
       <c r="J197" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.45">
@@ -25043,13 +25059,13 @@
         <v>390</v>
       </c>
       <c r="C198" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D198" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="E198" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="G198" s="7">
         <v>-30216.382900000001</v>
@@ -25061,7 +25077,7 @@
         <v>33</v>
       </c>
       <c r="J198" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K198" t="s">
         <v>349</v>
@@ -25075,13 +25091,13 @@
         <v>390</v>
       </c>
       <c r="C199" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D199" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E199" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G199" s="7">
         <v>-30401.414799999999</v>
@@ -25093,10 +25109,10 @@
         <v>33</v>
       </c>
       <c r="J199" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K199" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.45">
@@ -25110,7 +25126,7 @@
         <v>346</v>
       </c>
       <c r="D200" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="E200" t="s">
         <v>104</v>
@@ -25125,7 +25141,7 @@
         <v>33</v>
       </c>
       <c r="J200" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K200" t="s">
         <v>345</v>
@@ -25139,13 +25155,13 @@
         <v>390</v>
       </c>
       <c r="C201" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D201" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="E201" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="G201" s="7">
         <v>-24672.011399999999</v>
@@ -25157,10 +25173,10 @@
         <v>33</v>
       </c>
       <c r="J201" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K201" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.45">
@@ -25174,10 +25190,10 @@
         <v>259</v>
       </c>
       <c r="E202" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F202" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="G202" s="7">
         <v>26158.044693</v>
@@ -25189,7 +25205,7 @@
         <v>33</v>
       </c>
       <c r="J202" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K202" t="s">
         <v>260</v>
@@ -25206,10 +25222,10 @@
         <v>261</v>
       </c>
       <c r="E203" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="F203" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="G203" s="7">
         <v>26065.148562999999</v>
@@ -25221,7 +25237,7 @@
         <v>33</v>
       </c>
       <c r="J203" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K203" t="s">
         <v>262</v>
@@ -25238,10 +25254,10 @@
         <v>263</v>
       </c>
       <c r="E204" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F204" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="G204" s="7">
         <v>26116.073284999999</v>
@@ -25253,7 +25269,7 @@
         <v>33</v>
       </c>
       <c r="J204" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K204" t="s">
         <v>372</v>
@@ -25270,10 +25286,10 @@
         <v>264</v>
       </c>
       <c r="E205" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="F205" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="G205" s="7">
         <v>21795.243349</v>
@@ -25285,7 +25301,7 @@
         <v>33</v>
       </c>
       <c r="J205" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K205" t="s">
         <v>265</v>
@@ -25302,10 +25318,10 @@
         <v>266</v>
       </c>
       <c r="E206" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="F206" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="G206" s="7">
         <v>24700.341451</v>
@@ -25317,7 +25333,7 @@
         <v>33</v>
       </c>
       <c r="J206" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.45">
@@ -25346,7 +25362,7 @@
         <v>33</v>
       </c>
       <c r="J207" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K207" t="s">
         <v>268</v>
@@ -25363,10 +25379,10 @@
         <v>248</v>
       </c>
       <c r="D208" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E208" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="G208" s="7">
         <v>-5382.4546069999997</v>
@@ -25378,7 +25394,7 @@
         <v>33</v>
       </c>
       <c r="J208" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.45">
@@ -25392,10 +25408,10 @@
         <v>251</v>
       </c>
       <c r="D209" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="E209" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="G209" s="7">
         <v>-5863.5875050000004</v>
@@ -25407,7 +25423,7 @@
         <v>33</v>
       </c>
       <c r="J209" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K209" t="s">
         <v>252</v>
@@ -25421,16 +25437,16 @@
         <v>238</v>
       </c>
       <c r="C210" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D210" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E210" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="F210" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G210" s="7">
         <v>-6692</v>
@@ -25442,10 +25458,10 @@
         <v>33</v>
       </c>
       <c r="J210" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K210" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.45">
@@ -25459,10 +25475,10 @@
         <v>246</v>
       </c>
       <c r="D211" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="E211" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="G211" s="7">
         <v>-16184.035458</v>
@@ -25474,7 +25490,7 @@
         <v>33</v>
       </c>
       <c r="J211" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="K211" t="s">
         <v>247</v>
@@ -25491,10 +25507,10 @@
         <v>244</v>
       </c>
       <c r="D212" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="E212" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="G212" s="7">
         <v>-14821.784298</v>
@@ -25506,7 +25522,7 @@
         <v>33</v>
       </c>
       <c r="J212" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K212" t="s">
         <v>245</v>
@@ -25523,10 +25539,10 @@
         <v>241</v>
       </c>
       <c r="D213" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="E213" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="G213" s="7">
         <v>-17974.03659</v>
@@ -25538,7 +25554,7 @@
         <v>33</v>
       </c>
       <c r="J213" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K213" t="s">
         <v>242</v>
@@ -25555,10 +25571,10 @@
         <v>239</v>
       </c>
       <c r="D214" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="E214" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="G214" s="7">
         <v>-16699.671394000001</v>
@@ -25570,7 +25586,7 @@
         <v>33</v>
       </c>
       <c r="J214" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K214" t="s">
         <v>240</v>
@@ -25587,10 +25603,10 @@
         <v>249</v>
       </c>
       <c r="D215" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="E215" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="G215" s="7">
         <v>-15587.081733000001</v>
@@ -25602,7 +25618,7 @@
         <v>33</v>
       </c>
       <c r="J215" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K215" t="s">
         <v>250</v>
@@ -25619,10 +25635,10 @@
         <v>243</v>
       </c>
       <c r="D216" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E216" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="G216" s="7">
         <v>-14532.244757</v>
@@ -25634,7 +25650,7 @@
         <v>33</v>
       </c>
       <c r="J216" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="217" spans="1:11" x14ac:dyDescent="0.45">
@@ -25648,7 +25664,7 @@
         <v>255</v>
       </c>
       <c r="D217" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="E217" t="s">
         <v>256</v>
@@ -25663,7 +25679,7 @@
         <v>33</v>
       </c>
       <c r="J217" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K217" t="s">
         <v>371</v>
@@ -25680,7 +25696,7 @@
         <v>253</v>
       </c>
       <c r="D218" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="E218" t="s">
         <v>254</v>
@@ -25695,7 +25711,7 @@
         <v>33</v>
       </c>
       <c r="J218" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K218" t="s">
         <v>371</v>
@@ -25712,7 +25728,7 @@
         <v>257</v>
       </c>
       <c r="D219" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="E219" t="s">
         <v>258</v>
@@ -25727,7 +25743,7 @@
         <v>33</v>
       </c>
       <c r="J219" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K219" t="s">
         <v>371</v>
@@ -25741,6 +25757,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <gdc15e87e6184dc285cecc59dfe3e409 xmlns="99b93dda-0db1-4804-bcd9-79ac3408f7b3">
@@ -25777,16 +25802,12 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="f3010fb3-0ead-40f9-8418-3186255a05f9" ContentTypeId="0x010100D14BD004BF1C4459B890F3727F092580" PreviousValue="false"/>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Miljødirektoratet Dokument" ma:contentTypeID="0x010100D14BD004BF1C4459B890F3727F0925800030788E1E5F06E4499248722442C9E1E2" ma:contentTypeVersion="4" ma:contentTypeDescription="Opprett et nytt dokument. " ma:contentTypeScope="" ma:versionID="31d2f06e1319184035b49374dedadd14">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99b93dda-0db1-4804-bcd9-79ac3408f7b3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b39a69652e56cca026e8bfba402999b" ns2:_="">
     <xsd:import namespace="99b93dda-0db1-4804-bcd9-79ac3408f7b3"/>
@@ -25952,12 +25973,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="f3010fb3-0ead-40f9-8418-3186255a05f9" ContentTypeId="0x010100D14BD004BF1C4459B890F3727F092580" PreviousValue="false"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3C45CF2-DB67-4850-A387-8CB1B8396D69}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E2C70A-39DB-4E9F-AC55-CF83C6FAF41A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -25973,15 +25997,15 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3C45CF2-DB67-4850-A387-8CB1B8396D69}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{045B6229-1055-4164-AB1C-6A3398378E43}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{465F94C6-DADA-41F7-9419-4CB4FA36834F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25997,12 +26021,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{045B6229-1055-4164-AB1C-6A3398378E43}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>